<commit_message>
Large update of numerous files.
</commit_message>
<xml_diff>
--- a/python/tutorial organization file.xlsx
+++ b/python/tutorial organization file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bob\Documents\Extensive Enterprises\Mass Street University\Repos\MassStreetUniversity.github.io\src\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4da9f1820d624f37/Documents/Extensive Enterprises/Mass Street University/Repos/code-tutorial-source/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618B821F-3A18-4926-B934-84E844325AB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{618B821F-3A18-4926-B934-84E844325AB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F322C1FC-FE60-4DCC-B5E3-53E94E0678FB}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lessons" sheetId="4" r:id="rId1"/>
@@ -238,9 +238,6 @@
     <t>importing-modules</t>
   </si>
   <si>
-    <t>pep8</t>
-  </si>
-  <si>
     <t>Download Anaconda</t>
   </si>
   <si>
@@ -521,6 +518,9 @@
   </si>
   <si>
     <t>Lesson</t>
+  </si>
+  <si>
+    <t>python-programming-standards</t>
   </si>
 </sst>
 </file>
@@ -896,7 +896,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>47</v>
@@ -904,20 +904,20 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
         <v>135</v>
-      </c>
-      <c r="B4" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -930,8 +930,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,7 +955,7 @@
         <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -982,34 +982,34 @@
         <v>31</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E2" t="str">
         <f>"Section"&amp;" "&amp;C2&amp;"."&amp;" "&amp;D2</f>
         <v>Section I. A Note From The Author</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H2" s="8" t="str">
         <f t="shared" ref="H2:H13" si="0">F2&amp;"-"&amp;G2</f>
@@ -1034,26 +1034,26 @@
     </row>
     <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E13" si="4">"Section"&amp;" "&amp;C3&amp;"."&amp;" "&amp;D3</f>
         <v>Section II. Tutorial Overview</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H3" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1078,26 +1078,26 @@
     </row>
     <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="4"/>
         <v>Section III. What Is The Preflight Checklist?</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H4" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1122,26 +1122,26 @@
     </row>
     <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="4"/>
         <v>Section IV. Supplimentery Material</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H5" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1166,26 +1166,26 @@
     </row>
     <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="4"/>
         <v>Section V. Download Anaconda</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H6" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1210,26 +1210,26 @@
     </row>
     <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="4"/>
         <v>Section VI. Download PyCharm (Optional)</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H7" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1254,26 +1254,26 @@
     </row>
     <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="4"/>
         <v>Section VII. Download SQL Server Developer Edition</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H8" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1298,26 +1298,26 @@
     </row>
     <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="4"/>
         <v>Section VIII. Configure Database Environment</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H9" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1342,26 +1342,26 @@
     </row>
     <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="4"/>
         <v>Section IX. Download The Source Code</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H10" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1386,26 +1386,26 @@
     </row>
     <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="4"/>
         <v>Section X. Starting JupyterLab</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H11" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1430,26 +1430,26 @@
     </row>
     <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="4"/>
         <v>Section XI. Sign Up For Code Wars</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H12" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1474,26 +1474,26 @@
     </row>
     <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="4"/>
         <v>Section XII. How To Get Help With This Tutorial</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1516,12 +1516,12 @@
         <v>XII. &lt;a href="preflight/12-sos.html"&gt;How To Get Help With This Tutorial&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -1561,12 +1561,12 @@
         <v>1. &lt;a href="basics/01-hello-world.html"&gt;Obligatory Hello World&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C15" s="3">
         <f>C14+1</f>
@@ -1607,12 +1607,12 @@
         <v>2. &lt;a href="basics/02-code-comments.html"&gt;Code Comments&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" ref="C16:C51" si="12">C15+1</f>
@@ -1653,12 +1653,12 @@
         <v>3. &lt;a href="basics/03-data-types.html"&gt;Data Types&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="12"/>
@@ -1699,12 +1699,12 @@
         <v>4. &lt;a href="basics/04-variables.html"&gt;Variables&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="12"/>
@@ -1745,12 +1745,12 @@
         <v>5. &lt;a href="basics/05-string-concatenation.html"&gt;String Concatenation&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="12"/>
@@ -1791,12 +1791,12 @@
         <v>6. &lt;a href="basics/06-arithmetic-operators.html"&gt;Arithmetic Operators&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" si="12"/>
@@ -1837,12 +1837,12 @@
         <v>7. &lt;a href="basics/07-making-decisions.html"&gt;Making Decisions&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" si="12"/>
@@ -1883,12 +1883,12 @@
         <v>8. &lt;a href="basics/08-control-flow-if-else.html"&gt;Control Flow With if-elif-else&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" si="12"/>
@@ -1929,12 +1929,12 @@
         <v>9. &lt;a href="basics/09-control-flow-while.html"&gt;Control Flow With While&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" si="12"/>
@@ -1975,12 +1975,12 @@
         <v>10. &lt;a href="basics/10-list.html"&gt;Data Structures Part I: List&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" si="12"/>
@@ -2021,12 +2021,12 @@
         <v>11. &lt;a href="basics/11-tuples.html"&gt;Data Structures Part II: Tuples&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" si="12"/>
@@ -2067,12 +2067,12 @@
         <v>12. &lt;a href="basics/12-dictionaries.html"&gt;Data Structures Part III: Dictionaries&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C26" s="3">
         <f t="shared" si="12"/>
@@ -2113,12 +2113,12 @@
         <v>13. &lt;a href="basics/13-looping-with-for.html"&gt;Looping With for&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C27" s="3">
         <f t="shared" si="12"/>
@@ -2159,12 +2159,12 @@
         <v>14. &lt;a href="basics/14-functions.html"&gt;Functions&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C28" s="3">
         <f t="shared" si="12"/>
@@ -2205,12 +2205,12 @@
         <v>15. &lt;a href="basics/15-importing-modules.html"&gt;Importing Modules&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C29" s="3">
         <f t="shared" si="12"/>
@@ -2228,19 +2228,19 @@
         <v>16</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>65</v>
+        <v>159</v>
       </c>
       <c r="H29" s="8" t="str">
         <f t="shared" si="8"/>
-        <v>16-pep8</v>
+        <v>16-python-programming-standards</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="16"/>
-        <v>16-pep8.ipynb</v>
+        <v>16-python-programming-standards.ipynb</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="17"/>
-        <v>16-pep8.html</v>
+        <v>16-python-programming-standards.html</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="5"/>
@@ -2248,22 +2248,22 @@
       </c>
       <c r="L29" t="str">
         <f t="shared" si="11"/>
-        <v>16. &lt;a href="basics/16-pep8.html"&gt;Python Programming Standards&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>16. &lt;a href="basics/16-python-programming-standards.html"&gt;Python Programming Standards&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C30" s="3">
         <f t="shared" si="12"/>
         <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="6"/>
@@ -2297,12 +2297,12 @@
         <v>17. &lt;a href="advanced/17-map.html"&gt;Functional Programing With map&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C31" s="3">
         <f t="shared" si="12"/>
@@ -2343,12 +2343,12 @@
         <v>18. &lt;a href="advanced/18-generators.html"&gt;Generators&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C32" s="3">
         <f t="shared" si="12"/>
@@ -2389,19 +2389,19 @@
         <v>19. &lt;a href="advanced/19-comprehensions.html"&gt;Comprehensions&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C33" s="3">
         <f t="shared" si="12"/>
         <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="6"/>
@@ -2412,7 +2412,7 @@
         <v>20</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H33" s="8" t="str">
         <f t="shared" si="8"/>
@@ -2435,19 +2435,19 @@
         <v>20. &lt;a href="advanced/20-basic-file-operations.html"&gt;Basic File Operations&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C34" s="3">
         <f t="shared" si="12"/>
         <v>21</v>
       </c>
       <c r="D34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="6"/>
@@ -2458,7 +2458,7 @@
         <v>21</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H34" s="8" t="str">
         <f t="shared" si="8"/>
@@ -2481,12 +2481,12 @@
         <v>21. &lt;a href="advanced/21-numpy.html"&gt;Working With Data In NumPy&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C35" s="3">
         <f t="shared" si="12"/>
@@ -2504,7 +2504,7 @@
         <v>22</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H35" s="8" t="str">
         <f t="shared" ref="H35:H40" si="18">F35&amp;"-"&amp;G35</f>
@@ -2527,12 +2527,12 @@
         <v>22. &lt;a href="advanced/22-pandas.html"&gt;Working With Data In Pandas&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C36" s="3">
         <f t="shared" si="12"/>
@@ -2550,7 +2550,7 @@
         <v>23</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H36" s="8" t="str">
         <f t="shared" si="18"/>
@@ -2573,12 +2573,12 @@
         <v>23. &lt;a href="advanced/23-json.html"&gt;Working With JSON&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C37" s="3">
         <f t="shared" si="12"/>
@@ -2596,7 +2596,7 @@
         <v>24</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H37" s="8" t="str">
         <f t="shared" si="18"/>
@@ -2619,12 +2619,12 @@
         <v>24. &lt;a href="advanced/24-requesting-files-with-http-ftp.html"&gt;Making File Request Over HTTP And FTP&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C38" s="3">
         <f t="shared" si="12"/>
@@ -2642,7 +2642,7 @@
         <v>25</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H38" s="8" t="str">
         <f t="shared" si="18"/>
@@ -2665,19 +2665,19 @@
         <v>25. &lt;a href="advanced/25-databases.html"&gt;Interacting With Databases&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C39" s="3">
         <f t="shared" si="12"/>
         <v>26</v>
       </c>
       <c r="D39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="6"/>
@@ -2688,7 +2688,7 @@
         <v>26</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H39" s="8" t="str">
         <f t="shared" si="18"/>
@@ -2711,12 +2711,12 @@
         <v>26. &lt;a href="advanced/26-saving-objects-with-pickle.html"&gt;Saving Objects With Pickle&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C40" s="3">
         <f t="shared" si="12"/>
@@ -2734,7 +2734,7 @@
         <v>27</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H40" s="8" t="str">
         <f t="shared" si="18"/>
@@ -2757,19 +2757,19 @@
         <v>27. &lt;a href="advanced/27-error-handling.html"&gt;Error Handling&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C41" s="3">
         <f t="shared" si="12"/>
         <v>28</v>
       </c>
       <c r="D41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E41" t="str">
         <f>"Lesson"&amp;" "&amp;C41&amp;"."&amp;" "&amp;D41</f>
@@ -2780,7 +2780,7 @@
         <v>28</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H41" s="8" t="str">
         <f>F41&amp;"-"&amp;G41</f>
@@ -2808,14 +2808,14 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C42" s="3">
         <f t="shared" si="12"/>
         <v>29</v>
       </c>
       <c r="D42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" ref="E42:E51" si="22">"Lesson"&amp;" "&amp;C42&amp;"."&amp;" "&amp;D42</f>
@@ -2826,7 +2826,7 @@
         <v>29</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H42" s="8" t="str">
         <f t="shared" ref="H42:H45" si="23">F42&amp;"-"&amp;G42</f>
@@ -2854,7 +2854,7 @@
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C43" s="3">
         <f t="shared" si="12"/>
@@ -2872,7 +2872,7 @@
         <v>30</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H43" s="8" t="str">
         <f t="shared" si="23"/>
@@ -2900,14 +2900,14 @@
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C44" s="3">
         <f t="shared" si="12"/>
         <v>31</v>
       </c>
       <c r="D44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="22"/>
@@ -2918,7 +2918,7 @@
         <v>31</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H44" s="8" t="str">
         <f t="shared" si="23"/>
@@ -2946,14 +2946,14 @@
         <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C45" s="3">
         <f t="shared" si="12"/>
         <v>32</v>
       </c>
       <c r="D45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="22"/>
@@ -2964,7 +2964,7 @@
         <v>32</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H45" s="8" t="str">
         <f t="shared" si="23"/>
@@ -2992,14 +2992,14 @@
         <v>40</v>
       </c>
       <c r="B46" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C46" s="3">
         <f t="shared" si="12"/>
         <v>33</v>
       </c>
       <c r="D46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E46" t="str">
         <f>"Lesson"&amp;" "&amp;C46&amp;"."&amp;" "&amp;D46</f>
@@ -3010,7 +3010,7 @@
         <v>33</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H46" s="8" t="str">
         <f>F46&amp;"-"&amp;G46</f>
@@ -3038,14 +3038,14 @@
         <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C47" s="3">
         <f t="shared" si="12"/>
         <v>34</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="22"/>
@@ -3056,7 +3056,7 @@
         <v>34</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H47" s="8" t="str">
         <f t="shared" ref="H47:H51" si="27">F47&amp;"-"&amp;G47</f>
@@ -3084,14 +3084,14 @@
         <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C48" s="3">
         <f t="shared" si="12"/>
         <v>35</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="22"/>
@@ -3102,7 +3102,7 @@
         <v>35</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H48" s="8" t="str">
         <f t="shared" si="27"/>
@@ -3130,14 +3130,14 @@
         <v>40</v>
       </c>
       <c r="B49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C49" s="3">
         <f t="shared" si="12"/>
         <v>36</v>
       </c>
       <c r="D49" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="22"/>
@@ -3148,7 +3148,7 @@
         <v>36</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H49" s="8" t="str">
         <f t="shared" si="27"/>
@@ -3173,17 +3173,17 @@
     </row>
     <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C50" s="3">
         <f t="shared" si="12"/>
         <v>37</v>
       </c>
       <c r="D50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="22"/>
@@ -3194,7 +3194,7 @@
         <v>37</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H50" s="5" t="str">
         <f t="shared" si="27"/>
@@ -3219,17 +3219,17 @@
     </row>
     <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C51" s="3">
         <f t="shared" si="12"/>
         <v>38</v>
       </c>
       <c r="D51" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="22"/>
@@ -3240,7 +3240,7 @@
         <v>38</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H51" s="5" t="str">
         <f t="shared" si="27"/>
@@ -3267,7 +3267,7 @@
   <autoFilter ref="A1:L51" xr:uid="{C26BCB42-6FAD-4781-AC88-8DB659BD4328}">
     <filterColumn colId="0">
       <filters>
-        <filter val="basics"/>
+        <filter val="advanced"/>
       </filters>
     </filterColumn>
     <filterColumn colId="1">
@@ -3306,8 +3306,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02720D5E-A20F-4CFA-8B9E-1EE48C4E0140}">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4138,7 +4139,7 @@
       </c>
       <c r="E28" t="str">
         <f>'Lesson File Xref'!J29</f>
-        <v>16-pep8.html</v>
+        <v>16-python-programming-standards.html</v>
       </c>
       <c r="F28" s="4">
         <f>'Lesson File Xref'!C28</f>
@@ -4146,13 +4147,13 @@
       </c>
       <c r="G28" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/basics/14-functions.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/basics/16-pep8.html"&gt;Next&lt;/a&gt;</v>
+        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/basics/14-functions.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/basics/16-python-programming-standards.html"&gt;Next&lt;/a&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>'Lesson File Xref'!H29</f>
-        <v>16-pep8</v>
+        <v>16-python-programming-standards</v>
       </c>
       <c r="B29" t="str">
         <f>'Lesson File Xref'!A28</f>
@@ -4190,7 +4191,7 @@
       </c>
       <c r="C30" t="str">
         <f>'Lesson File Xref'!J29</f>
-        <v>16-pep8.html</v>
+        <v>16-python-programming-standards.html</v>
       </c>
       <c r="D30" t="str">
         <f>'Lesson File Xref'!A31</f>
@@ -4206,7 +4207,7 @@
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/basics/16-pep8.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/advanced/18-generators.html"&gt;Next&lt;/a&gt;</v>
+        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/basics/16-python-programming-standards.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/advanced/18-generators.html"&gt;Next&lt;/a&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -6721,7 +6722,7 @@
         <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -6729,7 +6730,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6737,7 +6738,7 @@
         <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6747,17 +6748,17 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a ton of random updates.
</commit_message>
<xml_diff>
--- a/python/tutorial organization file.xlsx
+++ b/python/tutorial organization file.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4da9f1820d624f37/Documents/Extensive Enterprises/Mass Street University/Repos/code-tutorial-source/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{618B821F-3A18-4926-B934-84E844325AB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F322C1FC-FE60-4DCC-B5E3-53E94E0678FB}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:1_{618B821F-3A18-4926-B934-84E844325AB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FA1CC0D8-C8CA-4E71-8F8F-E7E3A8914BCD}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lessons" sheetId="4" r:id="rId1"/>
     <sheet name="Lesson File Xref" sheetId="1" r:id="rId2"/>
-    <sheet name="Nav Link Builder" sheetId="2" r:id="rId3"/>
-    <sheet name="Has Table" sheetId="6" r:id="rId4"/>
-    <sheet name="Drop Down Values" sheetId="5" r:id="rId5"/>
+    <sheet name="Meta Tags" sheetId="7" r:id="rId3"/>
+    <sheet name="Nav Link Builder" sheetId="2" r:id="rId4"/>
+    <sheet name="Has Table" sheetId="6" r:id="rId5"/>
+    <sheet name="Drop Down Values" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Lesson File Xref'!$A$1:$L$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="176">
   <si>
     <t>Lesson Name</t>
   </si>
@@ -475,42 +475,6 @@
     <t>Repo File Name</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>09</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>Lesson Type</t>
   </si>
   <si>
@@ -521,13 +485,97 @@
   </si>
   <si>
     <t>python-programming-standards</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>ii</t>
+  </si>
+  <si>
+    <t>iii</t>
+  </si>
+  <si>
+    <t>iv</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>vi</t>
+  </si>
+  <si>
+    <t>vii</t>
+  </si>
+  <si>
+    <t>viii</t>
+  </si>
+  <si>
+    <t>ix</t>
+  </si>
+  <si>
+    <t>xi</t>
+  </si>
+  <si>
+    <t>xii</t>
+  </si>
+  <si>
+    <t>Lesson Specific Phrase</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>I explain my reasoning behind why I wrote a Python instead of an R tutorial.</t>
+  </si>
+  <si>
+    <t>I explain what we’re going to go over in this tutorial.</t>
+  </si>
+  <si>
+    <t>I explain what exactly the preflight checklist is.</t>
+  </si>
+  <si>
+    <t>I point out other MSDS resources for learning Python.</t>
+  </si>
+  <si>
+    <t>I show you where you can download the popular Python distribution known as Anaconda.</t>
+  </si>
+  <si>
+    <t>I show you where you can download a Python IDE if you’d prefer that instead of using notebook technology.</t>
+  </si>
+  <si>
+    <t>I show you where you can download SQL Server Developer Edition.</t>
+  </si>
+  <si>
+    <t>I tell you how to set up your development environment.</t>
+  </si>
+  <si>
+    <t>I show you were to download the source code for the examples.</t>
+  </si>
+  <si>
+    <t>I show you how to turn on JupyterLab because it’s not straight forward.</t>
+  </si>
+  <si>
+    <t>I introduce you to Code Wars where we’ll be offering extra training.</t>
+  </si>
+  <si>
+    <t>I show you the various ways you can get support for this tutorial.</t>
+  </si>
+  <si>
+    <t>I offer the standard Hello World lesson that is required of every code tutorial on planet Earth.</t>
+  </si>
+  <si>
+    <t>I teach you how to comment your code.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -539,6 +587,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -564,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -594,6 +649,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,11 +985,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,7 +1012,7 @@
         <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -988,12 +1045,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>110</v>
@@ -1006,38 +1063,38 @@
         <v>Section I. A Note From The Author</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>122</v>
       </c>
       <c r="H2" s="8" t="str">
         <f t="shared" ref="H2:H13" si="0">F2&amp;"-"&amp;G2</f>
-        <v>01-authors-note</v>
+        <v>i-authors-note</v>
       </c>
       <c r="I2" t="str">
         <f t="shared" ref="I2:I13" si="1">F2&amp;"-"&amp;G2&amp;".ipynb"</f>
-        <v>01-authors-note.ipynb</v>
+        <v>i-authors-note.ipynb</v>
       </c>
       <c r="J2" t="str">
         <f t="shared" ref="J2:J13" si="2">F2&amp;"-"&amp;G2&amp;".html"</f>
-        <v>01-authors-note.html</v>
+        <v>i-authors-note.html</v>
       </c>
       <c r="K2" t="str">
         <f>B2&amp;" "&amp;F2&amp;" "&amp;D2</f>
-        <v>Section 01 A Note From The Author</v>
+        <v>Section i A Note From The Author</v>
       </c>
       <c r="L2" t="str">
         <f t="shared" ref="L2:L13" si="3">C2&amp;". &lt;a href="""&amp;A2&amp;"/"&amp;J2&amp;"""&gt;"&amp;D2&amp;"&lt;/a&gt;"</f>
-        <v>I. &lt;a href="preface/01-authors-note.html"&gt;A Note From The Author&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>I. &lt;a href="preface/i-authors-note.html"&gt;A Note From The Author&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>111</v>
@@ -1050,38 +1107,38 @@
         <v>Section II. Tutorial Overview</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>123</v>
       </c>
       <c r="H3" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>02-overview</v>
+        <v>ii-overview</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="1"/>
-        <v>02-overview.ipynb</v>
+        <v>ii-overview.ipynb</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" si="2"/>
-        <v>02-overview.html</v>
+        <v>ii-overview.html</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" ref="K3:K51" si="5">B3&amp;" "&amp;F3&amp;" "&amp;D3</f>
-        <v>Section 02 Tutorial Overview</v>
+        <v>Section ii Tutorial Overview</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" si="3"/>
-        <v>II. &lt;a href="preface/02-overview.html"&gt;Tutorial Overview&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>II. &lt;a href="preface/ii-overview.html"&gt;Tutorial Overview&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>112</v>
@@ -1094,38 +1151,38 @@
         <v>Section III. What Is The Preflight Checklist?</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>124</v>
       </c>
       <c r="H4" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>03-what-is-the-checklist</v>
+        <v>iii-what-is-the-checklist</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="1"/>
-        <v>03-what-is-the-checklist.ipynb</v>
+        <v>iii-what-is-the-checklist.ipynb</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="2"/>
-        <v>03-what-is-the-checklist.html</v>
+        <v>iii-what-is-the-checklist.html</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="5"/>
-        <v>Section 03 What Is The Preflight Checklist?</v>
+        <v>Section iii What Is The Preflight Checklist?</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="3"/>
-        <v>III. &lt;a href="preface/03-what-is-the-checklist.html"&gt;What Is The Preflight Checklist?&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>III. &lt;a href="preface/iii-what-is-the-checklist.html"&gt;What Is The Preflight Checklist?&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>113</v>
@@ -1138,38 +1195,38 @@
         <v>Section IV. Supplimentery Material</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>125</v>
       </c>
       <c r="H5" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>04-swag</v>
+        <v>iv-swag</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="1"/>
-        <v>04-swag.ipynb</v>
+        <v>iv-swag.ipynb</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="2"/>
-        <v>04-swag.html</v>
+        <v>iv-swag.html</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="5"/>
-        <v>Section 04 Supplimentery Material</v>
+        <v>Section iv Supplimentery Material</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="3"/>
-        <v>IV. &lt;a href="preface/04-swag.html"&gt;Supplimentery Material&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>IV. &lt;a href="preface/iv-swag.html"&gt;Supplimentery Material&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>114</v>
@@ -1182,38 +1239,38 @@
         <v>Section V. Download Anaconda</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>126</v>
       </c>
       <c r="H6" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>05-anconda</v>
+        <v>v-anconda</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="1"/>
-        <v>05-anconda.ipynb</v>
+        <v>v-anconda.ipynb</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="2"/>
-        <v>05-anconda.html</v>
+        <v>v-anconda.html</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="5"/>
-        <v>Section 05 Download Anaconda</v>
+        <v>Section v Download Anaconda</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="3"/>
-        <v>V. &lt;a href="preflight/05-anconda.html"&gt;Download Anaconda&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>V. &lt;a href="preflight/v-anconda.html"&gt;Download Anaconda&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>115</v>
@@ -1226,38 +1283,38 @@
         <v>Section VI. Download PyCharm (Optional)</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>127</v>
       </c>
       <c r="H7" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>06-pycharm</v>
+        <v>vi-pycharm</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="1"/>
-        <v>06-pycharm.ipynb</v>
+        <v>vi-pycharm.ipynb</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="2"/>
-        <v>06-pycharm.html</v>
+        <v>vi-pycharm.html</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="5"/>
-        <v>Section 06 Download PyCharm (Optional)</v>
+        <v>Section vi Download PyCharm (Optional)</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="3"/>
-        <v>VI. &lt;a href="preflight/06-pycharm.html"&gt;Download PyCharm (Optional)&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>VI. &lt;a href="preflight/vi-pycharm.html"&gt;Download PyCharm (Optional)&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>109</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>116</v>
@@ -1270,38 +1327,38 @@
         <v>Section VII. Download SQL Server Developer Edition</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>128</v>
       </c>
       <c r="H8" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>07-sql-server</v>
+        <v>vii-sql-server</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="1"/>
-        <v>07-sql-server.ipynb</v>
+        <v>vii-sql-server.ipynb</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="2"/>
-        <v>07-sql-server.html</v>
+        <v>vii-sql-server.html</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="5"/>
-        <v>Section 07 Download SQL Server Developer Edition</v>
+        <v>Section vii Download SQL Server Developer Edition</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="3"/>
-        <v>VII. &lt;a href="preflight/07-sql-server.html"&gt;Download SQL Server Developer Edition&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>VII. &lt;a href="preflight/vii-sql-server.html"&gt;Download SQL Server Developer Edition&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>109</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>117</v>
@@ -1314,38 +1371,38 @@
         <v>Section VIII. Configure Database Environment</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>129</v>
       </c>
       <c r="H9" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>08-environment-setup</v>
+        <v>viii-environment-setup</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="1"/>
-        <v>08-environment-setup.ipynb</v>
+        <v>viii-environment-setup.ipynb</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="2"/>
-        <v>08-environment-setup.html</v>
+        <v>viii-environment-setup.html</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="5"/>
-        <v>Section 08 Configure Database Environment</v>
+        <v>Section viii Configure Database Environment</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="3"/>
-        <v>VIII. &lt;a href="preflight/08-environment-setup.html"&gt;Configure Database Environment&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>VIII. &lt;a href="preflight/viii-environment-setup.html"&gt;Configure Database Environment&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>118</v>
@@ -1358,38 +1415,38 @@
         <v>Section IX. Download The Source Code</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>130</v>
       </c>
       <c r="H10" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>09-source-code</v>
+        <v>ix-source-code</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="1"/>
-        <v>09-source-code.ipynb</v>
+        <v>ix-source-code.ipynb</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="2"/>
-        <v>09-source-code.html</v>
+        <v>ix-source-code.html</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="5"/>
-        <v>Section 09 Download The Source Code</v>
+        <v>Section ix Download The Source Code</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="3"/>
-        <v>IX. &lt;a href="preflight/09-source-code.html"&gt;Download The Source Code&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>IX. &lt;a href="preflight/ix-source-code.html"&gt;Download The Source Code&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>119</v>
@@ -1402,38 +1459,38 @@
         <v>Section X. Starting JupyterLab</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>131</v>
       </c>
       <c r="H11" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>10-starting-jupyterlab</v>
+        <v>xi-starting-jupyterlab</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="1"/>
-        <v>10-starting-jupyterlab.ipynb</v>
+        <v>xi-starting-jupyterlab.ipynb</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="2"/>
-        <v>10-starting-jupyterlab.html</v>
+        <v>xi-starting-jupyterlab.html</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="5"/>
-        <v>Section 10 Starting JupyterLab</v>
+        <v>Section xi Starting JupyterLab</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="3"/>
-        <v>X. &lt;a href="preflight/10-starting-jupyterlab.html"&gt;Starting JupyterLab&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>X. &lt;a href="preflight/xi-starting-jupyterlab.html"&gt;Starting JupyterLab&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>109</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>120</v>
@@ -1446,38 +1503,38 @@
         <v>Section XI. Sign Up For Code Wars</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>132</v>
       </c>
       <c r="H12" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>11-code-wars</v>
+        <v>xi-code-wars</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="1"/>
-        <v>11-code-wars.ipynb</v>
+        <v>xi-code-wars.ipynb</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="2"/>
-        <v>11-code-wars.html</v>
+        <v>xi-code-wars.html</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="5"/>
-        <v>Section 11 Sign Up For Code Wars</v>
+        <v>Section xi Sign Up For Code Wars</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="3"/>
-        <v>XI. &lt;a href="preflight/11-code-wars.html"&gt;Sign Up For Code Wars&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>XI. &lt;a href="preflight/xi-code-wars.html"&gt;Sign Up For Code Wars&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>109</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>121</v>
@@ -1490,38 +1547,38 @@
         <v>Section XII. How To Get Help With This Tutorial</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>133</v>
       </c>
       <c r="H13" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>12-sos</v>
+        <v>xii-sos</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="1"/>
-        <v>12-sos.ipynb</v>
+        <v>xii-sos.ipynb</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="2"/>
-        <v>12-sos.html</v>
+        <v>xii-sos.html</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="5"/>
-        <v>Section 12 How To Get Help With This Tutorial</v>
+        <v>Section xii How To Get Help With This Tutorial</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="3"/>
-        <v>XII. &lt;a href="preflight/12-sos.html"&gt;How To Get Help With This Tutorial&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>XII. &lt;a href="preflight/xii-sos.html"&gt;How To Get Help With This Tutorial&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -1561,12 +1618,12 @@
         <v>1. &lt;a href="basics/01-hello-world.html"&gt;Obligatory Hello World&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C15" s="3">
         <f>C14+1</f>
@@ -1607,12 +1664,12 @@
         <v>2. &lt;a href="basics/02-code-comments.html"&gt;Code Comments&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" ref="C16:C51" si="12">C15+1</f>
@@ -1653,12 +1710,12 @@
         <v>3. &lt;a href="basics/03-data-types.html"&gt;Data Types&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="12"/>
@@ -1699,12 +1756,12 @@
         <v>4. &lt;a href="basics/04-variables.html"&gt;Variables&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="12"/>
@@ -1745,12 +1802,12 @@
         <v>5. &lt;a href="basics/05-string-concatenation.html"&gt;String Concatenation&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="12"/>
@@ -1791,12 +1848,12 @@
         <v>6. &lt;a href="basics/06-arithmetic-operators.html"&gt;Arithmetic Operators&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" si="12"/>
@@ -1837,12 +1894,12 @@
         <v>7. &lt;a href="basics/07-making-decisions.html"&gt;Making Decisions&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" si="12"/>
@@ -1883,12 +1940,12 @@
         <v>8. &lt;a href="basics/08-control-flow-if-else.html"&gt;Control Flow With if-elif-else&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" si="12"/>
@@ -1929,12 +1986,12 @@
         <v>9. &lt;a href="basics/09-control-flow-while.html"&gt;Control Flow With While&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" si="12"/>
@@ -1975,12 +2032,12 @@
         <v>10. &lt;a href="basics/10-list.html"&gt;Data Structures Part I: List&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" si="12"/>
@@ -2021,12 +2078,12 @@
         <v>11. &lt;a href="basics/11-tuples.html"&gt;Data Structures Part II: Tuples&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" si="12"/>
@@ -2067,12 +2124,12 @@
         <v>12. &lt;a href="basics/12-dictionaries.html"&gt;Data Structures Part III: Dictionaries&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C26" s="3">
         <f t="shared" si="12"/>
@@ -2113,12 +2170,12 @@
         <v>13. &lt;a href="basics/13-looping-with-for.html"&gt;Looping With for&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C27" s="3">
         <f t="shared" si="12"/>
@@ -2159,12 +2216,12 @@
         <v>14. &lt;a href="basics/14-functions.html"&gt;Functions&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C28" s="3">
         <f t="shared" si="12"/>
@@ -2205,12 +2262,12 @@
         <v>15. &lt;a href="basics/15-importing-modules.html"&gt;Importing Modules&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C29" s="3">
         <f t="shared" si="12"/>
@@ -2228,7 +2285,7 @@
         <v>16</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="H29" s="8" t="str">
         <f t="shared" si="8"/>
@@ -2256,7 +2313,7 @@
         <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C30" s="3">
         <f t="shared" si="12"/>
@@ -2302,7 +2359,7 @@
         <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C31" s="3">
         <f t="shared" si="12"/>
@@ -2348,7 +2405,7 @@
         <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C32" s="3">
         <f t="shared" si="12"/>
@@ -2394,7 +2451,7 @@
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C33" s="3">
         <f t="shared" si="12"/>
@@ -2440,7 +2497,7 @@
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C34" s="3">
         <f t="shared" si="12"/>
@@ -2486,7 +2543,7 @@
         <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C35" s="3">
         <f t="shared" si="12"/>
@@ -2532,7 +2589,7 @@
         <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C36" s="3">
         <f t="shared" si="12"/>
@@ -2578,7 +2635,7 @@
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C37" s="3">
         <f t="shared" si="12"/>
@@ -2624,7 +2681,7 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C38" s="3">
         <f t="shared" si="12"/>
@@ -2670,7 +2727,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C39" s="3">
         <f t="shared" si="12"/>
@@ -2716,7 +2773,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C40" s="3">
         <f t="shared" si="12"/>
@@ -2762,7 +2819,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C41" s="3">
         <f t="shared" si="12"/>
@@ -2803,12 +2860,12 @@
         <v>28. &lt;a href="advanced/28-bringing-it-all-together.html"&gt;Bringing It All Together&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C42" s="3">
         <f t="shared" si="12"/>
@@ -2849,12 +2906,12 @@
         <v>29. &lt;a href="solutions/29-download-a-zip-file.html"&gt;Download A Zip File Over HTTP&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C43" s="3">
         <f t="shared" si="12"/>
@@ -2895,12 +2952,12 @@
         <v>30. &lt;a href="solutions/30-looping-over-files-in-a-directory.html"&gt;Looping Over Files In A Directory&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C44" s="3">
         <f t="shared" si="12"/>
@@ -2941,12 +2998,12 @@
         <v>31. &lt;a href="solutions/31-convert-file-to-pipe-delimited.html"&gt;Convert Comma Delmited Files To Pipe Delimited&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C45" s="3">
         <f t="shared" si="12"/>
@@ -2987,12 +3044,12 @@
         <v>32. &lt;a href="solutions/32-combine-csvs-into-one-file.html"&gt;Combining Multiple CSVs Into One File&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>40</v>
       </c>
       <c r="B46" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C46" s="3">
         <f t="shared" si="12"/>
@@ -3033,12 +3090,12 @@
         <v>33. &lt;a href="solutions/33-load-large-csvs-into-data-warehouse.html"&gt;Load Large CSVs Into Data Warehouse Staging Tables&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C47" s="3">
         <f t="shared" si="12"/>
@@ -3079,12 +3136,12 @@
         <v>34. &lt;a href="solutions/34-efficient-disk-write.html"&gt;Efficiently Write Large Database Query Results To Disk&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C48" s="3">
         <f t="shared" si="12"/>
@@ -3125,12 +3182,12 @@
         <v>35. &lt;a href="solutions/35-sftp-in-the-real-world.html"&gt;Working With SFTP In The Real World&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>40</v>
       </c>
       <c r="B49" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C49" s="3">
         <f t="shared" si="12"/>
@@ -3171,12 +3228,12 @@
         <v>36. &lt;a href="solutions/36-run-python-from-sql-server.html"&gt;Executing Python From SQL Server Agent&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C50" s="3">
         <f t="shared" si="12"/>
@@ -3217,12 +3274,12 @@
         <v>37. &lt;a href="project/37-final-project.html"&gt;Final Project&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>98</v>
       </c>
       <c r="B51" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C51" s="3">
         <f t="shared" si="12"/>
@@ -3264,23 +3321,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L51" xr:uid="{C26BCB42-6FAD-4781-AC88-8DB659BD4328}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="advanced"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Lesson"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L51" xr:uid="{C26BCB42-6FAD-4781-AC88-8DB659BD4328}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="F2:F13" numberStoredAsText="1"/>
-  </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -3303,12 +3346,958 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA4136B-2C83-4DC0-A4CA-D1A27C680A6D}">
+  <dimension ref="A1:E49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="98.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="96" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>'Lesson File Xref'!A2</f>
+        <v>preface</v>
+      </c>
+      <c r="B2" t="str">
+        <f>'Lesson File Xref'!E2</f>
+        <v>Section I. A Note From The Author</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" t="str">
+        <f>B2</f>
+        <v>Section I. A Note From The Author</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"In this section,"&amp;" "&amp;C2</f>
+        <v>In this section, I explain my reasoning behind why I wrote a Python instead of an R tutorial.</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>'Lesson File Xref'!A3</f>
+        <v>preface</v>
+      </c>
+      <c r="B3" t="str">
+        <f>'Lesson File Xref'!E3</f>
+        <v>Section II. Tutorial Overview</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D13" si="0">B3</f>
+        <v>Section II. Tutorial Overview</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E13" si="1">"In this section,"&amp;" "&amp;C3</f>
+        <v>In this section, I explain what we’re going to go over in this tutorial.</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>'Lesson File Xref'!A4</f>
+        <v>preface</v>
+      </c>
+      <c r="B4" t="str">
+        <f>'Lesson File Xref'!E4</f>
+        <v>Section III. What Is The Preflight Checklist?</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>Section III. What Is The Preflight Checklist?</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>In this section, I explain what exactly the preflight checklist is.</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>'Lesson File Xref'!A5</f>
+        <v>preface</v>
+      </c>
+      <c r="B5" t="str">
+        <f>'Lesson File Xref'!E5</f>
+        <v>Section IV. Supplimentery Material</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>Section IV. Supplimentery Material</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>In this section, I point out other MSDS resources for learning Python.</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>'Lesson File Xref'!A6</f>
+        <v>preflight</v>
+      </c>
+      <c r="B6" t="str">
+        <f>'Lesson File Xref'!E6</f>
+        <v>Section V. Download Anaconda</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>Section V. Download Anaconda</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>In this section, I show you where you can download the popular Python distribution known as Anaconda.</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>'Lesson File Xref'!A7</f>
+        <v>preflight</v>
+      </c>
+      <c r="B7" t="str">
+        <f>'Lesson File Xref'!E7</f>
+        <v>Section VI. Download PyCharm (Optional)</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>Section VI. Download PyCharm (Optional)</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>In this section, I show you where you can download a Python IDE if you’d prefer that instead of using notebook technology.</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>'Lesson File Xref'!A8</f>
+        <v>preflight</v>
+      </c>
+      <c r="B8" t="str">
+        <f>'Lesson File Xref'!E8</f>
+        <v>Section VII. Download SQL Server Developer Edition</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>Section VII. Download SQL Server Developer Edition</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>In this section, I show you where you can download SQL Server Developer Edition.</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>'Lesson File Xref'!A9</f>
+        <v>preflight</v>
+      </c>
+      <c r="B9" t="str">
+        <f>'Lesson File Xref'!E9</f>
+        <v>Section VIII. Configure Database Environment</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>Section VIII. Configure Database Environment</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>In this section, I tell you how to set up your development environment.</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>'Lesson File Xref'!A10</f>
+        <v>preflight</v>
+      </c>
+      <c r="B10" t="str">
+        <f>'Lesson File Xref'!E10</f>
+        <v>Section IX. Download The Source Code</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>Section IX. Download The Source Code</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>In this section, I show you were to download the source code for the examples.</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>'Lesson File Xref'!A11</f>
+        <v>preflight</v>
+      </c>
+      <c r="B11" t="str">
+        <f>'Lesson File Xref'!E11</f>
+        <v>Section X. Starting JupyterLab</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>Section X. Starting JupyterLab</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>In this section, I show you how to turn on JupyterLab because it’s not straight forward.</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>'Lesson File Xref'!A12</f>
+        <v>preflight</v>
+      </c>
+      <c r="B12" t="str">
+        <f>'Lesson File Xref'!E12</f>
+        <v>Section XI. Sign Up For Code Wars</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>Section XI. Sign Up For Code Wars</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>In this section, I introduce you to Code Wars where we’ll be offering extra training.</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f>'Lesson File Xref'!A13</f>
+        <v>preflight</v>
+      </c>
+      <c r="B13" t="str">
+        <f>'Lesson File Xref'!E13</f>
+        <v>Section XII. How To Get Help With This Tutorial</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>Section XII. How To Get Help With This Tutorial</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>In this section, I show you the various ways you can get support for this tutorial.</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>'Lesson File Xref'!A14</f>
+        <v>basics</v>
+      </c>
+      <c r="B14" t="str">
+        <f>'Lesson File Xref'!E14</f>
+        <v>Lesson 1. Obligatory Hello World</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" ref="D3:D66" si="2">B14&amp;" "&amp;"With Python"</f>
+        <v>Lesson 1. Obligatory Hello World With Python</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" ref="E3:E66" si="3">"In this lesson,"&amp;" "&amp;C14</f>
+        <v>In this lesson, I offer the standard Hello World lesson that is required of every code tutorial on planet Earth.</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>'Lesson File Xref'!A15</f>
+        <v>basics</v>
+      </c>
+      <c r="B15" t="str">
+        <f>'Lesson File Xref'!E15</f>
+        <v>Lesson 2. Code Comments</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 2. Code Comments With Python</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="3"/>
+        <v>In this lesson, I teach you how to comment your code.</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f>'Lesson File Xref'!A16</f>
+        <v>basics</v>
+      </c>
+      <c r="B16" t="str">
+        <f>'Lesson File Xref'!E16</f>
+        <v>Lesson 3. Data Types</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 3. Data Types With Python</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>'Lesson File Xref'!A17</f>
+        <v>basics</v>
+      </c>
+      <c r="B17" t="str">
+        <f>'Lesson File Xref'!E17</f>
+        <v>Lesson 4. Variables</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 4. Variables With Python</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>'Lesson File Xref'!A18</f>
+        <v>basics</v>
+      </c>
+      <c r="B18" t="str">
+        <f>'Lesson File Xref'!E18</f>
+        <v>Lesson 5. String Concatenation</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 5. String Concatenation With Python</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>'Lesson File Xref'!A19</f>
+        <v>basics</v>
+      </c>
+      <c r="B19" t="str">
+        <f>'Lesson File Xref'!E19</f>
+        <v>Lesson 6. Arithmetic Operators</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 6. Arithmetic Operators With Python</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>'Lesson File Xref'!A20</f>
+        <v>basics</v>
+      </c>
+      <c r="B20" t="str">
+        <f>'Lesson File Xref'!E20</f>
+        <v>Lesson 7. Making Decisions</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 7. Making Decisions With Python</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>'Lesson File Xref'!A21</f>
+        <v>basics</v>
+      </c>
+      <c r="B21" t="str">
+        <f>'Lesson File Xref'!E21</f>
+        <v>Lesson 8. Control Flow With if-elif-else</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 8. Control Flow With if-elif-else With Python</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f>'Lesson File Xref'!A22</f>
+        <v>basics</v>
+      </c>
+      <c r="B22" t="str">
+        <f>'Lesson File Xref'!E22</f>
+        <v>Lesson 9. Control Flow With While</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 9. Control Flow With While With Python</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f>'Lesson File Xref'!A23</f>
+        <v>basics</v>
+      </c>
+      <c r="B23" t="str">
+        <f>'Lesson File Xref'!E23</f>
+        <v>Lesson 10. Data Structures Part I: List</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 10. Data Structures Part I: List With Python</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>'Lesson File Xref'!A24</f>
+        <v>basics</v>
+      </c>
+      <c r="B24" t="str">
+        <f>'Lesson File Xref'!E24</f>
+        <v>Lesson 11. Data Structures Part II: Tuples</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 11. Data Structures Part II: Tuples With Python</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>'Lesson File Xref'!A25</f>
+        <v>basics</v>
+      </c>
+      <c r="B25" t="str">
+        <f>'Lesson File Xref'!E25</f>
+        <v>Lesson 12. Data Structures Part III: Dictionaries</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 12. Data Structures Part III: Dictionaries With Python</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>'Lesson File Xref'!A26</f>
+        <v>basics</v>
+      </c>
+      <c r="B26" t="str">
+        <f>'Lesson File Xref'!E26</f>
+        <v>Lesson 13. Looping With for</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 13. Looping With for With Python</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>'Lesson File Xref'!A27</f>
+        <v>basics</v>
+      </c>
+      <c r="B27" t="str">
+        <f>'Lesson File Xref'!E27</f>
+        <v>Lesson 14. Functions</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 14. Functions With Python</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>'Lesson File Xref'!A28</f>
+        <v>basics</v>
+      </c>
+      <c r="B28" t="str">
+        <f>'Lesson File Xref'!E28</f>
+        <v>Lesson 15. Importing Modules</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 15. Importing Modules With Python</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f>'Lesson File Xref'!A29</f>
+        <v>basics</v>
+      </c>
+      <c r="B29" t="str">
+        <f>'Lesson File Xref'!E29</f>
+        <v>Lesson 16. Python Programming Standards</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 16. Python Programming Standards With Python</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f>'Lesson File Xref'!A30</f>
+        <v>advanced</v>
+      </c>
+      <c r="B30" t="str">
+        <f>'Lesson File Xref'!E30</f>
+        <v>Lesson 17. Functional Programing With map</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 17. Functional Programing With map With Python</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f>'Lesson File Xref'!A31</f>
+        <v>advanced</v>
+      </c>
+      <c r="B31" t="str">
+        <f>'Lesson File Xref'!E31</f>
+        <v>Lesson 18. Generators</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 18. Generators With Python</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f>'Lesson File Xref'!A32</f>
+        <v>advanced</v>
+      </c>
+      <c r="B32" t="str">
+        <f>'Lesson File Xref'!E32</f>
+        <v>Lesson 19. Comprehensions</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 19. Comprehensions With Python</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>'Lesson File Xref'!A33</f>
+        <v>advanced</v>
+      </c>
+      <c r="B33" t="str">
+        <f>'Lesson File Xref'!E33</f>
+        <v>Lesson 20. Basic File Operations</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 20. Basic File Operations With Python</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f>'Lesson File Xref'!A34</f>
+        <v>advanced</v>
+      </c>
+      <c r="B34" t="str">
+        <f>'Lesson File Xref'!E34</f>
+        <v>Lesson 21. Working With Data In NumPy</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 21. Working With Data In NumPy With Python</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f>'Lesson File Xref'!A35</f>
+        <v>advanced</v>
+      </c>
+      <c r="B35" t="str">
+        <f>'Lesson File Xref'!E35</f>
+        <v>Lesson 22. Working With Data In Pandas</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 22. Working With Data In Pandas With Python</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f>'Lesson File Xref'!A36</f>
+        <v>advanced</v>
+      </c>
+      <c r="B36" t="str">
+        <f>'Lesson File Xref'!E36</f>
+        <v>Lesson 23. Working With JSON</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 23. Working With JSON With Python</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f>'Lesson File Xref'!A37</f>
+        <v>advanced</v>
+      </c>
+      <c r="B37" t="str">
+        <f>'Lesson File Xref'!E37</f>
+        <v>Lesson 24. Making File Request Over HTTP And FTP</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 24. Making File Request Over HTTP And FTP With Python</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f>'Lesson File Xref'!A38</f>
+        <v>advanced</v>
+      </c>
+      <c r="B38" t="str">
+        <f>'Lesson File Xref'!E38</f>
+        <v>Lesson 25. Interacting With Databases</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 25. Interacting With Databases With Python</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f>'Lesson File Xref'!A39</f>
+        <v>advanced</v>
+      </c>
+      <c r="B39" t="str">
+        <f>'Lesson File Xref'!E39</f>
+        <v>Lesson 26. Saving Objects With Pickle</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 26. Saving Objects With Pickle With Python</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f>'Lesson File Xref'!A40</f>
+        <v>advanced</v>
+      </c>
+      <c r="B40" t="str">
+        <f>'Lesson File Xref'!E40</f>
+        <v>Lesson 27. Error Handling</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 27. Error Handling With Python</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="str">
+        <f>'Lesson File Xref'!A41</f>
+        <v>advanced</v>
+      </c>
+      <c r="B41" t="str">
+        <f>'Lesson File Xref'!E41</f>
+        <v>Lesson 28. Bringing It All Together</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 28. Bringing It All Together With Python</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f>'Lesson File Xref'!A42</f>
+        <v>solutions</v>
+      </c>
+      <c r="B42" t="str">
+        <f>'Lesson File Xref'!E42</f>
+        <v>Lesson 29. Download A Zip File Over HTTP</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 29. Download A Zip File Over HTTP With Python</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="str">
+        <f>'Lesson File Xref'!A43</f>
+        <v>solutions</v>
+      </c>
+      <c r="B43" t="str">
+        <f>'Lesson File Xref'!E43</f>
+        <v>Lesson 30. Looping Over Files In A Directory</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 30. Looping Over Files In A Directory With Python</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="str">
+        <f>'Lesson File Xref'!A44</f>
+        <v>solutions</v>
+      </c>
+      <c r="B44" t="str">
+        <f>'Lesson File Xref'!E44</f>
+        <v>Lesson 31. Convert Comma Delmited Files To Pipe Delimited</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 31. Convert Comma Delmited Files To Pipe Delimited With Python</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
+        <f>'Lesson File Xref'!A45</f>
+        <v>solutions</v>
+      </c>
+      <c r="B45" t="str">
+        <f>'Lesson File Xref'!E45</f>
+        <v>Lesson 32. Combining Multiple CSVs Into One File</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 32. Combining Multiple CSVs Into One File With Python</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
+        <f>'Lesson File Xref'!A46</f>
+        <v>solutions</v>
+      </c>
+      <c r="B46" t="str">
+        <f>'Lesson File Xref'!E46</f>
+        <v>Lesson 33. Load Large CSVs Into Data Warehouse Staging Tables</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 33. Load Large CSVs Into Data Warehouse Staging Tables With Python</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="str">
+        <f>'Lesson File Xref'!A47</f>
+        <v>solutions</v>
+      </c>
+      <c r="B47" t="str">
+        <f>'Lesson File Xref'!E47</f>
+        <v>Lesson 34. Efficiently Write Large Database Query Results To Disk</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 34. Efficiently Write Large Database Query Results To Disk With Python</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="str">
+        <f>'Lesson File Xref'!A48</f>
+        <v>solutions</v>
+      </c>
+      <c r="B48" t="str">
+        <f>'Lesson File Xref'!E48</f>
+        <v>Lesson 35. Working With SFTP In The Real World</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 35. Working With SFTP In The Real World With Python</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="str">
+        <f>'Lesson File Xref'!A49</f>
+        <v>solutions</v>
+      </c>
+      <c r="B49" t="str">
+        <f>'Lesson File Xref'!E49</f>
+        <v>Lesson 36. Executing Python From SQL Server Agent</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="2"/>
+        <v>Lesson 36. Executing Python From SQL Server Agent With Python</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">In this lesson, </v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02720D5E-A20F-4CFA-8B9E-1EE48C4E0140}">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3317,9 +4306,9 @@
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3349,7 +4338,7 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'Lesson File Xref'!H2</f>
-        <v>01-authors-note</v>
+        <v>i-authors-note</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3359,7 +4348,7 @@
       </c>
       <c r="E2" t="str">
         <f>'Lesson File Xref'!J3</f>
-        <v>02-overview.html</v>
+        <v>ii-overview.html</v>
       </c>
       <c r="F2" s="4" t="str">
         <f>'Lesson File Xref'!C2</f>
@@ -3367,13 +4356,13 @@
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G13" si="0">"&lt;a href=""https://tutorials.massstreetuniversity.com/python/""&gt;Tutorial Home&lt;/a&gt;"&amp;" | "&amp;"&lt;a href=""https://tutorials.massstreetuniversity.com/python/"&amp;B2&amp;"/"&amp;C2&amp;"""&gt;Previous&lt;/a&gt;"&amp;" | "&amp;"&lt;a href=""https://tutorials.massstreetuniversity.com/python/"&amp;D2&amp;"/"&amp;E2&amp;"""&gt;Next&lt;/a&gt;"</f>
-        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python//"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preface/02-overview.html"&gt;Next&lt;/a&gt;</v>
+        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python//"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preface/ii-overview.html"&gt;Next&lt;/a&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>'Lesson File Xref'!H3</f>
-        <v>02-overview</v>
+        <v>ii-overview</v>
       </c>
       <c r="B3" t="str">
         <f>'Lesson File Xref'!A2</f>
@@ -3381,7 +4370,7 @@
       </c>
       <c r="C3" t="str">
         <f>'Lesson File Xref'!J2</f>
-        <v>01-authors-note.html</v>
+        <v>i-authors-note.html</v>
       </c>
       <c r="D3" t="str">
         <f>'Lesson File Xref'!A4</f>
@@ -3389,7 +4378,7 @@
       </c>
       <c r="E3" t="str">
         <f>'Lesson File Xref'!J4</f>
-        <v>03-what-is-the-checklist.html</v>
+        <v>iii-what-is-the-checklist.html</v>
       </c>
       <c r="F3" s="4" t="str">
         <f>'Lesson File Xref'!C3</f>
@@ -3397,13 +4386,13 @@
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preface/01-authors-note.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preface/03-what-is-the-checklist.html"&gt;Next&lt;/a&gt;</v>
+        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preface/i-authors-note.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preface/iii-what-is-the-checklist.html"&gt;Next&lt;/a&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'Lesson File Xref'!H4</f>
-        <v>03-what-is-the-checklist</v>
+        <v>iii-what-is-the-checklist</v>
       </c>
       <c r="B4" t="str">
         <f>'Lesson File Xref'!A3</f>
@@ -3411,7 +4400,7 @@
       </c>
       <c r="C4" t="str">
         <f>'Lesson File Xref'!J3</f>
-        <v>02-overview.html</v>
+        <v>ii-overview.html</v>
       </c>
       <c r="D4" t="str">
         <f>'Lesson File Xref'!A5</f>
@@ -3419,7 +4408,7 @@
       </c>
       <c r="E4" t="str">
         <f>'Lesson File Xref'!J5</f>
-        <v>04-swag.html</v>
+        <v>iv-swag.html</v>
       </c>
       <c r="F4" s="4" t="str">
         <f>'Lesson File Xref'!C4</f>
@@ -3427,13 +4416,13 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preface/02-overview.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preface/04-swag.html"&gt;Next&lt;/a&gt;</v>
+        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preface/ii-overview.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preface/iv-swag.html"&gt;Next&lt;/a&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>'Lesson File Xref'!H5</f>
-        <v>04-swag</v>
+        <v>iv-swag</v>
       </c>
       <c r="B5" t="str">
         <f>'Lesson File Xref'!A4</f>
@@ -3441,7 +4430,7 @@
       </c>
       <c r="C5" t="str">
         <f>'Lesson File Xref'!J4</f>
-        <v>03-what-is-the-checklist.html</v>
+        <v>iii-what-is-the-checklist.html</v>
       </c>
       <c r="D5" t="str">
         <f>'Lesson File Xref'!A6</f>
@@ -3449,7 +4438,7 @@
       </c>
       <c r="E5" t="str">
         <f>'Lesson File Xref'!J6</f>
-        <v>05-anconda.html</v>
+        <v>v-anconda.html</v>
       </c>
       <c r="F5" s="4" t="str">
         <f>'Lesson File Xref'!C5</f>
@@ -3457,13 +4446,13 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preface/03-what-is-the-checklist.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/05-anconda.html"&gt;Next&lt;/a&gt;</v>
+        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preface/iii-what-is-the-checklist.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/v-anconda.html"&gt;Next&lt;/a&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>'Lesson File Xref'!H6</f>
-        <v>05-anconda</v>
+        <v>v-anconda</v>
       </c>
       <c r="B6" t="str">
         <f>'Lesson File Xref'!A5</f>
@@ -3471,7 +4460,7 @@
       </c>
       <c r="C6" t="str">
         <f>'Lesson File Xref'!J5</f>
-        <v>04-swag.html</v>
+        <v>iv-swag.html</v>
       </c>
       <c r="D6" t="str">
         <f>'Lesson File Xref'!A7</f>
@@ -3479,7 +4468,7 @@
       </c>
       <c r="E6" t="str">
         <f>'Lesson File Xref'!J7</f>
-        <v>06-pycharm.html</v>
+        <v>vi-pycharm.html</v>
       </c>
       <c r="F6" s="4" t="str">
         <f>'Lesson File Xref'!C6</f>
@@ -3487,13 +4476,13 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preface/04-swag.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/06-pycharm.html"&gt;Next&lt;/a&gt;</v>
+        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preface/iv-swag.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/vi-pycharm.html"&gt;Next&lt;/a&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>'Lesson File Xref'!H7</f>
-        <v>06-pycharm</v>
+        <v>vi-pycharm</v>
       </c>
       <c r="B7" t="str">
         <f>'Lesson File Xref'!A6</f>
@@ -3501,7 +4490,7 @@
       </c>
       <c r="C7" t="str">
         <f>'Lesson File Xref'!J6</f>
-        <v>05-anconda.html</v>
+        <v>v-anconda.html</v>
       </c>
       <c r="D7" t="str">
         <f>'Lesson File Xref'!A8</f>
@@ -3509,7 +4498,7 @@
       </c>
       <c r="E7" t="str">
         <f>'Lesson File Xref'!J8</f>
-        <v>07-sql-server.html</v>
+        <v>vii-sql-server.html</v>
       </c>
       <c r="F7" s="4" t="str">
         <f>'Lesson File Xref'!C7</f>
@@ -3517,13 +4506,13 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/05-anconda.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/07-sql-server.html"&gt;Next&lt;/a&gt;</v>
+        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/v-anconda.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/vii-sql-server.html"&gt;Next&lt;/a&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>'Lesson File Xref'!H8</f>
-        <v>07-sql-server</v>
+        <v>vii-sql-server</v>
       </c>
       <c r="B8" t="str">
         <f>'Lesson File Xref'!A7</f>
@@ -3531,7 +4520,7 @@
       </c>
       <c r="C8" t="str">
         <f>'Lesson File Xref'!J7</f>
-        <v>06-pycharm.html</v>
+        <v>vi-pycharm.html</v>
       </c>
       <c r="D8" t="str">
         <f>'Lesson File Xref'!A9</f>
@@ -3539,7 +4528,7 @@
       </c>
       <c r="E8" t="str">
         <f>'Lesson File Xref'!J9</f>
-        <v>08-environment-setup.html</v>
+        <v>viii-environment-setup.html</v>
       </c>
       <c r="F8" s="4" t="str">
         <f>'Lesson File Xref'!C8</f>
@@ -3547,13 +4536,13 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/06-pycharm.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/08-environment-setup.html"&gt;Next&lt;/a&gt;</v>
+        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/vi-pycharm.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/viii-environment-setup.html"&gt;Next&lt;/a&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>'Lesson File Xref'!H9</f>
-        <v>08-environment-setup</v>
+        <v>viii-environment-setup</v>
       </c>
       <c r="B9" t="str">
         <f>'Lesson File Xref'!A8</f>
@@ -3561,7 +4550,7 @@
       </c>
       <c r="C9" t="str">
         <f>'Lesson File Xref'!J8</f>
-        <v>07-sql-server.html</v>
+        <v>vii-sql-server.html</v>
       </c>
       <c r="D9" t="str">
         <f>'Lesson File Xref'!A10</f>
@@ -3569,7 +4558,7 @@
       </c>
       <c r="E9" t="str">
         <f>'Lesson File Xref'!J10</f>
-        <v>09-source-code.html</v>
+        <v>ix-source-code.html</v>
       </c>
       <c r="F9" s="4" t="str">
         <f>'Lesson File Xref'!C9</f>
@@ -3577,13 +4566,13 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/07-sql-server.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/09-source-code.html"&gt;Next&lt;/a&gt;</v>
+        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/vii-sql-server.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/ix-source-code.html"&gt;Next&lt;/a&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>'Lesson File Xref'!H10</f>
-        <v>09-source-code</v>
+        <v>ix-source-code</v>
       </c>
       <c r="B10" t="str">
         <f>'Lesson File Xref'!A9</f>
@@ -3591,7 +4580,7 @@
       </c>
       <c r="C10" t="str">
         <f>'Lesson File Xref'!J9</f>
-        <v>08-environment-setup.html</v>
+        <v>viii-environment-setup.html</v>
       </c>
       <c r="D10" t="str">
         <f>'Lesson File Xref'!A11</f>
@@ -3599,7 +4588,7 @@
       </c>
       <c r="E10" t="str">
         <f>'Lesson File Xref'!J11</f>
-        <v>10-starting-jupyterlab.html</v>
+        <v>xi-starting-jupyterlab.html</v>
       </c>
       <c r="F10" s="4" t="str">
         <f>'Lesson File Xref'!C10</f>
@@ -3607,13 +4596,13 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/08-environment-setup.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/10-starting-jupyterlab.html"&gt;Next&lt;/a&gt;</v>
+        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/viii-environment-setup.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/xi-starting-jupyterlab.html"&gt;Next&lt;/a&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>'Lesson File Xref'!H11</f>
-        <v>10-starting-jupyterlab</v>
+        <v>xi-starting-jupyterlab</v>
       </c>
       <c r="B11" t="str">
         <f>'Lesson File Xref'!A10</f>
@@ -3621,7 +4610,7 @@
       </c>
       <c r="C11" t="str">
         <f>'Lesson File Xref'!J10</f>
-        <v>09-source-code.html</v>
+        <v>ix-source-code.html</v>
       </c>
       <c r="D11" t="str">
         <f>'Lesson File Xref'!A12</f>
@@ -3629,7 +4618,7 @@
       </c>
       <c r="E11" t="str">
         <f>'Lesson File Xref'!J12</f>
-        <v>11-code-wars.html</v>
+        <v>xi-code-wars.html</v>
       </c>
       <c r="F11" s="4" t="str">
         <f>'Lesson File Xref'!C11</f>
@@ -3637,13 +4626,13 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/09-source-code.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/11-code-wars.html"&gt;Next&lt;/a&gt;</v>
+        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/ix-source-code.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/xi-code-wars.html"&gt;Next&lt;/a&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>'Lesson File Xref'!H12</f>
-        <v>11-code-wars</v>
+        <v>xi-code-wars</v>
       </c>
       <c r="B12" t="str">
         <f>'Lesson File Xref'!A11</f>
@@ -3651,7 +4640,7 @@
       </c>
       <c r="C12" t="str">
         <f>'Lesson File Xref'!J11</f>
-        <v>10-starting-jupyterlab.html</v>
+        <v>xi-starting-jupyterlab.html</v>
       </c>
       <c r="D12" t="str">
         <f>'Lesson File Xref'!A13</f>
@@ -3659,7 +4648,7 @@
       </c>
       <c r="E12" t="str">
         <f>'Lesson File Xref'!J13</f>
-        <v>12-sos.html</v>
+        <v>xii-sos.html</v>
       </c>
       <c r="F12" s="4" t="str">
         <f>'Lesson File Xref'!C12</f>
@@ -3667,13 +4656,13 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/10-starting-jupyterlab.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/12-sos.html"&gt;Next&lt;/a&gt;</v>
+        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/xi-starting-jupyterlab.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/xii-sos.html"&gt;Next&lt;/a&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>'Lesson File Xref'!H13</f>
-        <v>12-sos</v>
+        <v>xii-sos</v>
       </c>
       <c r="B13" t="str">
         <f>'Lesson File Xref'!A12</f>
@@ -3681,7 +4670,7 @@
       </c>
       <c r="C13" t="str">
         <f>'Lesson File Xref'!J12</f>
-        <v>11-code-wars.html</v>
+        <v>xi-code-wars.html</v>
       </c>
       <c r="D13" t="str">
         <f>'Lesson File Xref'!A14</f>
@@ -3697,7 +4686,7 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/11-code-wars.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/basics/01-hello-world.html"&gt;Next&lt;/a&gt;</v>
+        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/xi-code-wars.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/basics/01-hello-world.html"&gt;Next&lt;/a&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3711,7 +4700,7 @@
       </c>
       <c r="C14" t="str">
         <f>'Lesson File Xref'!J13</f>
-        <v>12-sos.html</v>
+        <v>xii-sos.html</v>
       </c>
       <c r="D14" t="str">
         <f>'Lesson File Xref'!A15</f>
@@ -3727,7 +4716,7 @@
       </c>
       <c r="G14" t="str">
         <f>"&lt;a href=""https://tutorials.massstreetuniversity.com/python/""&gt;Tutorial Home&lt;/a&gt;"&amp;" | "&amp;"&lt;a href=""https://tutorials.massstreetuniversity.com/python/"&amp;B14&amp;"/"&amp;C14&amp;"""&gt;Previous&lt;/a&gt;"&amp;" | "&amp;"&lt;a href=""https://tutorials.massstreetuniversity.com/python/"&amp;D14&amp;"/"&amp;E14&amp;"""&gt;Next&lt;/a&gt;"</f>
-        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/12-sos.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/basics/02-code-comments.html"&gt;Next&lt;/a&gt;</v>
+        <v>&lt;a href="https://tutorials.massstreetuniversity.com/python/"&gt;Tutorial Home&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/preflight/xii-sos.html"&gt;Previous&lt;/a&gt; | &lt;a href="https://tutorials.massstreetuniversity.com/python/basics/02-code-comments.html"&gt;Next&lt;/a&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -6675,7 +7664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294EA8A1-0E7E-44A0-A6A4-77513EA2BCD5}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -6703,7 +7692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E2A746-8891-4393-B508-2B889EC92277}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -6722,7 +7711,7 @@
         <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -6730,7 +7719,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6738,7 +7727,7 @@
         <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Massive update of everything cause I'm lazy about committing code
</commit_message>
<xml_diff>
--- a/python/tutorial organization file.xlsx
+++ b/python/tutorial organization file.xlsx
@@ -1,29 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4da9f1820d624f37/Documents/Extensive Enterprises/Mass Street University/Repos/code-tutorial-source/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:1_{618B821F-3A18-4926-B934-84E844325AB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FA1CC0D8-C8CA-4E71-8F8F-E7E3A8914BCD}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="13_ncr:1_{618B821F-3A18-4926-B934-84E844325AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA399D31-0DFA-4F56-AD26-3ADF60FA53D2}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="26325" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lessons" sheetId="4" r:id="rId1"/>
     <sheet name="Lesson File Xref" sheetId="1" r:id="rId2"/>
     <sheet name="Meta Tags" sheetId="7" r:id="rId3"/>
-    <sheet name="Nav Link Builder" sheetId="2" r:id="rId4"/>
-    <sheet name="Has Table" sheetId="6" r:id="rId5"/>
-    <sheet name="Drop Down Values" sheetId="5" r:id="rId6"/>
+    <sheet name="Twitter Post Helper" sheetId="8" r:id="rId4"/>
+    <sheet name="Nav Link Builder" sheetId="2" r:id="rId5"/>
+    <sheet name="Has Table" sheetId="6" r:id="rId6"/>
+    <sheet name="Drop Down Values" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Lesson File Xref'!$A$1:$L$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Lesson File Xref'!$A$1:$M$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="215">
   <si>
     <t>Lesson Name</t>
   </si>
@@ -569,6 +571,123 @@
   </si>
   <si>
     <t>I teach you how to comment your code.</t>
+  </si>
+  <si>
+    <t>I teach you the different kinds of data types in Python!</t>
+  </si>
+  <si>
+    <t>I teach you how to work with variables!</t>
+  </si>
+  <si>
+    <t>I teach you how to smoosh stuff together!</t>
+  </si>
+  <si>
+    <t>I teach you how to do third grade math with code!</t>
+  </si>
+  <si>
+    <t>I'm going to show you the 10 different methods to make decisions with code!</t>
+  </si>
+  <si>
+    <t>I teach you how to control your roll!</t>
+  </si>
+  <si>
+    <t>we talk about talk about controlling flow again but this time, it's gonna take a while!</t>
+  </si>
+  <si>
+    <t>we talk about list!</t>
+  </si>
+  <si>
+    <t>we talk about tuples!</t>
+  </si>
+  <si>
+    <t>we talk about dictionaries!</t>
+  </si>
+  <si>
+    <t>we get loopy!</t>
+  </si>
+  <si>
+    <t>we out here trying to function!</t>
+  </si>
+  <si>
+    <t>I show you the true power of Python. Importing Modules!</t>
+  </si>
+  <si>
+    <t>we grow some self respect and get some standards as software engineers!</t>
+  </si>
+  <si>
+    <t>we explore the alternative paradigm to object oriented programming. Functional programming!</t>
+  </si>
+  <si>
+    <t>we'll be generating some discussion about generators!</t>
+  </si>
+  <si>
+    <t>you're going to understand the words that are coming out of my mouth! (Comprehension. Get it?)</t>
+  </si>
+  <si>
+    <t>it's ok to be basic because we're going to talk about how to work with files.</t>
+  </si>
+  <si>
+    <t>I'll give you an intro to Pandas's less attractive cousin.</t>
+  </si>
+  <si>
+    <t>you'll be sad to discover that you won't be working with cute bears.</t>
+  </si>
+  <si>
+    <t>you'll learn why JSON is everything XML was SUPPOSED to be.</t>
+  </si>
+  <si>
+    <t>we'll learn how to transfer files with various internet protocols.</t>
+  </si>
+  <si>
+    <t>we're gonna be all "SELECT * FROM" as we learn to get data from databases!</t>
+  </si>
+  <si>
+    <t>you're going to blow your grandma's mind when you tell her you learned how to pickle something!</t>
+  </si>
+  <si>
+    <t>I teach you how to deal with the crazy things users like to do to your code.</t>
+  </si>
+  <si>
+    <t>we're going to integrate all of the concepts we spoke about into a single concept.</t>
+  </si>
+  <si>
+    <t>we get into tips, tricks, and tactics. This is how I get zip files over the internet. It's harder than you think!</t>
+  </si>
+  <si>
+    <t>you'll learn a better file delimiter than the comma.</t>
+  </si>
+  <si>
+    <t>I teach you how to take a bunch of little files and make one big file which comes in handy when loading database tables.</t>
+  </si>
+  <si>
+    <t>I teach you how to write a large file to disk quickly!</t>
+  </si>
+  <si>
+    <t>I teach you how to use PowerShell to run your Python scripts from SQL Server.</t>
+  </si>
+  <si>
+    <t>you finally get to see why building ETL with SSIS packages is dumb. I mean, there is just no other word for it.</t>
+  </si>
+  <si>
+    <t>I teach you another highly efficient method of loading flat files into tables.</t>
+  </si>
+  <si>
+    <t>lower case title</t>
+  </si>
+  <si>
+    <t>Intro</t>
+  </si>
+  <si>
+    <t>Complete text</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Final Post</t>
+  </si>
+  <si>
+    <t>Social URL</t>
   </si>
 </sst>
 </file>
@@ -619,7 +738,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -652,6 +771,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -985,10 +1105,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,10 +1124,11 @@
     <col min="9" max="9" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="99" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="90.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="99" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1042,10 +1163,13 @@
         <v>143</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -1085,11 +1209,15 @@
         <v>Section i A Note From The Author</v>
       </c>
       <c r="L2" t="str">
-        <f t="shared" ref="L2:L13" si="3">C2&amp;". &lt;a href="""&amp;A2&amp;"/"&amp;J2&amp;"""&gt;"&amp;D2&amp;"&lt;/a&gt;"</f>
+        <f>"https://learn.massstreet.net/python/"&amp;A2&amp;"/"&amp;J2</f>
+        <v>https://learn.massstreet.net/python/preface/i-authors-note.html</v>
+      </c>
+      <c r="M2" t="str">
+        <f t="shared" ref="M2:M13" si="3">C2&amp;". &lt;a href="""&amp;A2&amp;"/"&amp;J2&amp;"""&gt;"&amp;D2&amp;"&lt;/a&gt;"</f>
         <v>I. &lt;a href="preface/i-authors-note.html"&gt;A Note From The Author&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -1129,11 +1257,15 @@
         <v>Section ii Tutorial Overview</v>
       </c>
       <c r="L3" t="str">
+        <f t="shared" ref="L3:L51" si="6">"https://learn.massstreet.net/python/"&amp;A3&amp;"/"&amp;J3</f>
+        <v>https://learn.massstreet.net/python/preface/ii-overview.html</v>
+      </c>
+      <c r="M3" t="str">
         <f t="shared" si="3"/>
         <v>II. &lt;a href="preface/ii-overview.html"&gt;Tutorial Overview&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -1173,11 +1305,15 @@
         <v>Section iii What Is The Preflight Checklist?</v>
       </c>
       <c r="L4" t="str">
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/preface/iii-what-is-the-checklist.html</v>
+      </c>
+      <c r="M4" t="str">
         <f t="shared" si="3"/>
         <v>III. &lt;a href="preface/iii-what-is-the-checklist.html"&gt;What Is The Preflight Checklist?&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -1217,11 +1353,15 @@
         <v>Section iv Supplimentery Material</v>
       </c>
       <c r="L5" t="str">
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/preface/iv-swag.html</v>
+      </c>
+      <c r="M5" t="str">
         <f t="shared" si="3"/>
         <v>IV. &lt;a href="preface/iv-swag.html"&gt;Supplimentery Material&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>109</v>
       </c>
@@ -1261,11 +1401,15 @@
         <v>Section v Download Anaconda</v>
       </c>
       <c r="L6" t="str">
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/preflight/v-anconda.html</v>
+      </c>
+      <c r="M6" t="str">
         <f t="shared" si="3"/>
         <v>V. &lt;a href="preflight/v-anconda.html"&gt;Download Anaconda&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -1305,11 +1449,15 @@
         <v>Section vi Download PyCharm (Optional)</v>
       </c>
       <c r="L7" t="str">
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/preflight/vi-pycharm.html</v>
+      </c>
+      <c r="M7" t="str">
         <f t="shared" si="3"/>
         <v>VI. &lt;a href="preflight/vi-pycharm.html"&gt;Download PyCharm (Optional)&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>109</v>
       </c>
@@ -1349,11 +1497,15 @@
         <v>Section vii Download SQL Server Developer Edition</v>
       </c>
       <c r="L8" t="str">
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/preflight/vii-sql-server.html</v>
+      </c>
+      <c r="M8" t="str">
         <f t="shared" si="3"/>
         <v>VII. &lt;a href="preflight/vii-sql-server.html"&gt;Download SQL Server Developer Edition&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>109</v>
       </c>
@@ -1393,11 +1545,15 @@
         <v>Section viii Configure Database Environment</v>
       </c>
       <c r="L9" t="str">
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/preflight/viii-environment-setup.html</v>
+      </c>
+      <c r="M9" t="str">
         <f t="shared" si="3"/>
         <v>VIII. &lt;a href="preflight/viii-environment-setup.html"&gt;Configure Database Environment&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>109</v>
       </c>
@@ -1437,11 +1593,15 @@
         <v>Section ix Download The Source Code</v>
       </c>
       <c r="L10" t="str">
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/preflight/ix-source-code.html</v>
+      </c>
+      <c r="M10" t="str">
         <f t="shared" si="3"/>
         <v>IX. &lt;a href="preflight/ix-source-code.html"&gt;Download The Source Code&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>109</v>
       </c>
@@ -1481,11 +1641,15 @@
         <v>Section xi Starting JupyterLab</v>
       </c>
       <c r="L11" t="str">
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/preflight/xi-starting-jupyterlab.html</v>
+      </c>
+      <c r="M11" t="str">
         <f t="shared" si="3"/>
         <v>X. &lt;a href="preflight/xi-starting-jupyterlab.html"&gt;Starting JupyterLab&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>109</v>
       </c>
@@ -1525,11 +1689,15 @@
         <v>Section xi Sign Up For Code Wars</v>
       </c>
       <c r="L12" t="str">
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/preflight/xi-code-wars.html</v>
+      </c>
+      <c r="M12" t="str">
         <f t="shared" si="3"/>
         <v>XI. &lt;a href="preflight/xi-code-wars.html"&gt;Sign Up For Code Wars&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -1569,11 +1737,15 @@
         <v>Section xii How To Get Help With This Tutorial</v>
       </c>
       <c r="L13" t="str">
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/preflight/xii-sos.html</v>
+      </c>
+      <c r="M13" t="str">
         <f t="shared" si="3"/>
         <v>XII. &lt;a href="preflight/xii-sos.html"&gt;How To Get Help With This Tutorial&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1614,11 +1786,15 @@
         <v>Lesson 01 Obligatory Hello World</v>
       </c>
       <c r="L14" t="str">
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/basics/01-hello-world.html</v>
+      </c>
+      <c r="M14" t="str">
         <f>C14&amp;". &lt;a href="""&amp;A14&amp;"/"&amp;J14&amp;"""&gt;"&amp;D14&amp;"&lt;/a&gt;"</f>
         <v>1. &lt;a href="basics/01-hello-world.html"&gt;Obligatory Hello World&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1633,26 +1809,26 @@
         <v>4</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" ref="E15:E40" si="6">"Lesson"&amp;" "&amp;C15&amp;"."&amp;" "&amp;D15</f>
+        <f t="shared" ref="E15:E40" si="7">"Lesson"&amp;" "&amp;C15&amp;"."&amp;" "&amp;D15</f>
         <v>Lesson 2. Code Comments</v>
       </c>
       <c r="F15" s="6" t="str">
-        <f t="shared" ref="F15:F39" si="7">IF(C15&lt;10,"0"&amp;C15,C15)</f>
+        <f t="shared" ref="F15:F39" si="8">IF(C15&lt;10,"0"&amp;C15,C15)</f>
         <v>02</v>
       </c>
       <c r="G15" t="s">
         <v>33</v>
       </c>
       <c r="H15" s="8" t="str">
-        <f t="shared" ref="H15:H34" si="8">F15&amp;"-"&amp;G15</f>
+        <f t="shared" ref="H15:H34" si="9">F15&amp;"-"&amp;G15</f>
         <v>02-code-comments</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" ref="I15:I27" si="9">F15&amp;"-"&amp;G15&amp;".ipynb"</f>
+        <f t="shared" ref="I15:I27" si="10">F15&amp;"-"&amp;G15&amp;".ipynb"</f>
         <v>02-code-comments.ipynb</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" ref="J15:J27" si="10">F15&amp;"-"&amp;G15&amp;".html"</f>
+        <f t="shared" ref="J15:J27" si="11">F15&amp;"-"&amp;G15&amp;".html"</f>
         <v>02-code-comments.html</v>
       </c>
       <c r="K15" t="str">
@@ -1660,11 +1836,15 @@
         <v>Lesson 02 Code Comments</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" ref="L15:L40" si="11">C15&amp;". &lt;a href="""&amp;A15&amp;"/"&amp;J15&amp;"""&gt;"&amp;D15&amp;"&lt;/a&gt;"</f>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/basics/02-code-comments.html</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" ref="M15:M40" si="12">C15&amp;". &lt;a href="""&amp;A15&amp;"/"&amp;J15&amp;"""&gt;"&amp;D15&amp;"&lt;/a&gt;"</f>
         <v>2. &lt;a href="basics/02-code-comments.html"&gt;Code Comments&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1672,33 +1852,33 @@
         <v>146</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" ref="C16:C51" si="12">C15+1</f>
+        <f t="shared" ref="C16:C51" si="13">C15+1</f>
         <v>3</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 3. Data Types</v>
       </c>
       <c r="F16" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03</v>
       </c>
       <c r="G16" t="s">
         <v>35</v>
       </c>
       <c r="H16" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>03-data-types</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>03-data-types.ipynb</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>03-data-types.html</v>
       </c>
       <c r="K16" t="str">
@@ -1706,11 +1886,15 @@
         <v>Lesson 03 Data Types</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/basics/03-data-types.html</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="12"/>
         <v>3. &lt;a href="basics/03-data-types.html"&gt;Data Types&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1718,33 +1902,33 @@
         <v>146</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 4. Variables</v>
       </c>
       <c r="F17" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>04</v>
       </c>
       <c r="G17" t="s">
         <v>34</v>
       </c>
       <c r="H17" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>04-variables</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>04-variables.ipynb</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>04-variables.html</v>
       </c>
       <c r="K17" t="str">
@@ -1752,11 +1936,15 @@
         <v>Lesson 04 Variables</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/basics/04-variables.html</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="12"/>
         <v>4. &lt;a href="basics/04-variables.html"&gt;Variables&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1764,33 +1952,33 @@
         <v>146</v>
       </c>
       <c r="C18" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 5. String Concatenation</v>
       </c>
       <c r="F18" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>05</v>
       </c>
       <c r="G18" t="s">
         <v>36</v>
       </c>
       <c r="H18" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>05-string-concatenation</v>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>05-string-concatenation.ipynb</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>05-string-concatenation.html</v>
       </c>
       <c r="K18" t="str">
@@ -1798,11 +1986,15 @@
         <v>Lesson 05 String Concatenation</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/basics/05-string-concatenation.html</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="12"/>
         <v>5. &lt;a href="basics/05-string-concatenation.html"&gt;String Concatenation&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1810,33 +2002,33 @@
         <v>146</v>
       </c>
       <c r="C19" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 6. Arithmetic Operators</v>
       </c>
       <c r="F19" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>06</v>
       </c>
       <c r="G19" t="s">
         <v>37</v>
       </c>
       <c r="H19" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>06-arithmetic-operators</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>06-arithmetic-operators.ipynb</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>06-arithmetic-operators.html</v>
       </c>
       <c r="K19" t="str">
@@ -1844,11 +2036,15 @@
         <v>Lesson 06 Arithmetic Operators</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/basics/06-arithmetic-operators.html</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="12"/>
         <v>6. &lt;a href="basics/06-arithmetic-operators.html"&gt;Arithmetic Operators&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1856,33 +2052,33 @@
         <v>146</v>
       </c>
       <c r="C20" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="D20" t="s">
         <v>50</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 7. Making Decisions</v>
       </c>
       <c r="F20" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>07</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>51</v>
       </c>
       <c r="H20" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>07-making-decisions</v>
       </c>
       <c r="I20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>07-making-decisions.ipynb</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>07-making-decisions.html</v>
       </c>
       <c r="K20" t="str">
@@ -1890,11 +2086,15 @@
         <v>Lesson 07 Making Decisions</v>
       </c>
       <c r="L20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/basics/07-making-decisions.html</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="12"/>
         <v>7. &lt;a href="basics/07-making-decisions.html"&gt;Making Decisions&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1902,33 +2102,33 @@
         <v>146</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 8. Control Flow With if-elif-else</v>
       </c>
       <c r="F21" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>08</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>48</v>
       </c>
       <c r="H21" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>08-control-flow-if-else</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>08-control-flow-if-else.ipynb</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>08-control-flow-if-else.html</v>
       </c>
       <c r="K21" t="str">
@@ -1936,11 +2136,15 @@
         <v>Lesson 08 Control Flow With if-elif-else</v>
       </c>
       <c r="L21" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/basics/08-control-flow-if-else.html</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="12"/>
         <v>8. &lt;a href="basics/08-control-flow-if-else.html"&gt;Control Flow With if-elif-else&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1948,33 +2152,33 @@
         <v>146</v>
       </c>
       <c r="C22" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>9</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 9. Control Flow With While</v>
       </c>
       <c r="F22" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>09</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>49</v>
       </c>
       <c r="H22" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>09-control-flow-while</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>09-control-flow-while.ipynb</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>09-control-flow-while.html</v>
       </c>
       <c r="K22" t="str">
@@ -1982,11 +2186,15 @@
         <v>Lesson 09 Control Flow With While</v>
       </c>
       <c r="L22" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/basics/09-control-flow-while.html</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="12"/>
         <v>9. &lt;a href="basics/09-control-flow-while.html"&gt;Control Flow With While&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1994,33 +2202,33 @@
         <v>146</v>
       </c>
       <c r="C23" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>10</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 10. Data Structures Part I: List</v>
       </c>
       <c r="F23" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>55</v>
       </c>
       <c r="H23" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10-list</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>10-list.ipynb</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10-list.html</v>
       </c>
       <c r="K23" t="str">
@@ -2028,11 +2236,15 @@
         <v>Lesson 10 Data Structures Part I: List</v>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/basics/10-list.html</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="12"/>
         <v>10. &lt;a href="basics/10-list.html"&gt;Data Structures Part I: List&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -2040,33 +2252,33 @@
         <v>146</v>
       </c>
       <c r="C24" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 11. Data Structures Part II: Tuples</v>
       </c>
       <c r="F24" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>57</v>
       </c>
       <c r="H24" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>11-tuples</v>
       </c>
       <c r="I24" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11-tuples.ipynb</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>11-tuples.html</v>
       </c>
       <c r="K24" t="str">
@@ -2074,11 +2286,15 @@
         <v>Lesson 11 Data Structures Part II: Tuples</v>
       </c>
       <c r="L24" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/basics/11-tuples.html</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="12"/>
         <v>11. &lt;a href="basics/11-tuples.html"&gt;Data Structures Part II: Tuples&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -2086,33 +2302,33 @@
         <v>146</v>
       </c>
       <c r="C25" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>12</v>
       </c>
       <c r="D25" t="s">
         <v>3</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 12. Data Structures Part III: Dictionaries</v>
       </c>
       <c r="F25" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>58</v>
       </c>
       <c r="H25" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>12-dictionaries</v>
       </c>
       <c r="I25" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12-dictionaries.ipynb</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>12-dictionaries.html</v>
       </c>
       <c r="K25" t="str">
@@ -2120,11 +2336,15 @@
         <v>Lesson 12 Data Structures Part III: Dictionaries</v>
       </c>
       <c r="L25" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/basics/12-dictionaries.html</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="12"/>
         <v>12. &lt;a href="basics/12-dictionaries.html"&gt;Data Structures Part III: Dictionaries&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -2132,33 +2352,33 @@
         <v>146</v>
       </c>
       <c r="C26" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>13</v>
       </c>
       <c r="D26" t="s">
         <v>56</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 13. Looping With for</v>
       </c>
       <c r="F26" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>59</v>
       </c>
       <c r="H26" s="8" t="str">
-        <f t="shared" ref="H26" si="13">F26&amp;"-"&amp;G26</f>
+        <f t="shared" ref="H26" si="14">F26&amp;"-"&amp;G26</f>
         <v>13-looping-with-for</v>
       </c>
       <c r="I26" t="str">
-        <f t="shared" ref="I26" si="14">F26&amp;"-"&amp;G26&amp;".ipynb"</f>
+        <f t="shared" ref="I26" si="15">F26&amp;"-"&amp;G26&amp;".ipynb"</f>
         <v>13-looping-with-for.ipynb</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" ref="J26" si="15">F26&amp;"-"&amp;G26&amp;".html"</f>
+        <f t="shared" ref="J26" si="16">F26&amp;"-"&amp;G26&amp;".html"</f>
         <v>13-looping-with-for.html</v>
       </c>
       <c r="K26" t="str">
@@ -2166,11 +2386,15 @@
         <v>Lesson 13 Looping With for</v>
       </c>
       <c r="L26" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/basics/13-looping-with-for.html</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="12"/>
         <v>13. &lt;a href="basics/13-looping-with-for.html"&gt;Looping With for&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2178,33 +2402,33 @@
         <v>146</v>
       </c>
       <c r="C27" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>14</v>
       </c>
       <c r="D27" t="s">
         <v>13</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 14. Functions</v>
       </c>
       <c r="F27" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>60</v>
       </c>
       <c r="H27" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>14-functions</v>
       </c>
       <c r="I27" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>14-functions.ipynb</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>14-functions.html</v>
       </c>
       <c r="K27" t="str">
@@ -2212,11 +2436,15 @@
         <v>Lesson 14 Functions</v>
       </c>
       <c r="L27" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/basics/14-functions.html</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="12"/>
         <v>14. &lt;a href="basics/14-functions.html"&gt;Functions&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2224,33 +2452,33 @@
         <v>146</v>
       </c>
       <c r="C28" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>15</v>
       </c>
       <c r="D28" t="s">
         <v>23</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 15. Importing Modules</v>
       </c>
       <c r="F28" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>64</v>
       </c>
       <c r="H28" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>15-importing-modules</v>
       </c>
       <c r="I28" t="str">
-        <f t="shared" ref="I28:I34" si="16">F28&amp;"-"&amp;G28&amp;".ipynb"</f>
+        <f t="shared" ref="I28:I34" si="17">F28&amp;"-"&amp;G28&amp;".ipynb"</f>
         <v>15-importing-modules.ipynb</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" ref="J28:J34" si="17">F28&amp;"-"&amp;G28&amp;".html"</f>
+        <f t="shared" ref="J28:J34" si="18">F28&amp;"-"&amp;G28&amp;".html"</f>
         <v>15-importing-modules.html</v>
       </c>
       <c r="K28" t="str">
@@ -2258,11 +2486,15 @@
         <v>Lesson 15 Importing Modules</v>
       </c>
       <c r="L28" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/basics/15-importing-modules.html</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="12"/>
         <v>15. &lt;a href="basics/15-importing-modules.html"&gt;Importing Modules&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2270,33 +2502,33 @@
         <v>146</v>
       </c>
       <c r="C29" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>16</v>
       </c>
       <c r="D29" t="s">
         <v>22</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 16. Python Programming Standards</v>
       </c>
       <c r="F29" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>147</v>
       </c>
       <c r="H29" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>16-python-programming-standards</v>
       </c>
       <c r="I29" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>16-python-programming-standards.ipynb</v>
       </c>
       <c r="J29" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>16-python-programming-standards.html</v>
       </c>
       <c r="K29" t="str">
@@ -2304,11 +2536,15 @@
         <v>Lesson 16 Python Programming Standards</v>
       </c>
       <c r="L29" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/basics/16-python-programming-standards.html</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="12"/>
         <v>16. &lt;a href="basics/16-python-programming-standards.html"&gt;Python Programming Standards&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -2316,33 +2552,33 @@
         <v>146</v>
       </c>
       <c r="C30" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17</v>
       </c>
       <c r="D30" t="s">
         <v>79</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 17. Functional Programing With map</v>
       </c>
       <c r="F30" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>61</v>
       </c>
       <c r="H30" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>17-map</v>
       </c>
       <c r="I30" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>17-map.ipynb</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>17-map.html</v>
       </c>
       <c r="K30" t="str">
@@ -2350,11 +2586,15 @@
         <v>Lesson 17 Functional Programing With map</v>
       </c>
       <c r="L30" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/advanced/17-map.html</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="12"/>
         <v>17. &lt;a href="advanced/17-map.html"&gt;Functional Programing With map&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -2362,33 +2602,33 @@
         <v>146</v>
       </c>
       <c r="C31" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>18</v>
       </c>
       <c r="D31" t="s">
         <v>15</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 18. Generators</v>
       </c>
       <c r="F31" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>62</v>
       </c>
       <c r="H31" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>18-generators</v>
       </c>
       <c r="I31" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>18-generators.ipynb</v>
       </c>
       <c r="J31" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>18-generators.html</v>
       </c>
       <c r="K31" t="str">
@@ -2396,11 +2636,15 @@
         <v>Lesson 18 Generators</v>
       </c>
       <c r="L31" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/advanced/18-generators.html</v>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" si="12"/>
         <v>18. &lt;a href="advanced/18-generators.html"&gt;Generators&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -2408,33 +2652,33 @@
         <v>146</v>
       </c>
       <c r="C32" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>19</v>
       </c>
       <c r="D32" t="s">
         <v>14</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 19. Comprehensions</v>
       </c>
       <c r="F32" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>63</v>
       </c>
       <c r="H32" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>19-comprehensions</v>
       </c>
       <c r="I32" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>19-comprehensions.ipynb</v>
       </c>
       <c r="J32" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>19-comprehensions.html</v>
       </c>
       <c r="K32" t="str">
@@ -2442,11 +2686,15 @@
         <v>Lesson 19 Comprehensions</v>
       </c>
       <c r="L32" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/advanced/19-comprehensions.html</v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="12"/>
         <v>19. &lt;a href="advanced/19-comprehensions.html"&gt;Comprehensions&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -2454,33 +2702,33 @@
         <v>146</v>
       </c>
       <c r="C33" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>20</v>
       </c>
       <c r="D33" t="s">
         <v>89</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 20. Basic File Operations</v>
       </c>
       <c r="F33" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>90</v>
       </c>
       <c r="H33" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>20-basic-file-operations</v>
       </c>
       <c r="I33" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>20-basic-file-operations.ipynb</v>
       </c>
       <c r="J33" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>20-basic-file-operations.html</v>
       </c>
       <c r="K33" t="str">
@@ -2488,11 +2736,15 @@
         <v>Lesson 20 Basic File Operations</v>
       </c>
       <c r="L33" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/advanced/20-basic-file-operations.html</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="12"/>
         <v>20. &lt;a href="advanced/20-basic-file-operations.html"&gt;Basic File Operations&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -2500,33 +2752,33 @@
         <v>146</v>
       </c>
       <c r="C34" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>21</v>
       </c>
       <c r="D34" t="s">
         <v>75</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 21. Working With Data In NumPy</v>
       </c>
       <c r="F34" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>76</v>
       </c>
       <c r="H34" s="8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>21-numpy</v>
       </c>
       <c r="I34" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>21-numpy.ipynb</v>
       </c>
       <c r="J34" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>21-numpy.html</v>
       </c>
       <c r="K34" t="str">
@@ -2534,11 +2786,15 @@
         <v>Lesson 21 Working With Data In NumPy</v>
       </c>
       <c r="L34" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/advanced/21-numpy.html</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="12"/>
         <v>21. &lt;a href="advanced/21-numpy.html"&gt;Working With Data In NumPy&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -2546,33 +2802,33 @@
         <v>146</v>
       </c>
       <c r="C35" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>22</v>
       </c>
       <c r="D35" t="s">
         <v>18</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 22. Working With Data In Pandas</v>
       </c>
       <c r="F35" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>70</v>
       </c>
       <c r="H35" s="8" t="str">
-        <f t="shared" ref="H35:H40" si="18">F35&amp;"-"&amp;G35</f>
+        <f t="shared" ref="H35:H40" si="19">F35&amp;"-"&amp;G35</f>
         <v>22-pandas</v>
       </c>
       <c r="I35" t="str">
-        <f t="shared" ref="I35:I40" si="19">F35&amp;"-"&amp;G35&amp;".ipynb"</f>
+        <f t="shared" ref="I35:I40" si="20">F35&amp;"-"&amp;G35&amp;".ipynb"</f>
         <v>22-pandas.ipynb</v>
       </c>
       <c r="J35" t="str">
-        <f t="shared" ref="J35:J40" si="20">F35&amp;"-"&amp;G35&amp;".html"</f>
+        <f t="shared" ref="J35:J40" si="21">F35&amp;"-"&amp;G35&amp;".html"</f>
         <v>22-pandas.html</v>
       </c>
       <c r="K35" t="str">
@@ -2580,11 +2836,15 @@
         <v>Lesson 22 Working With Data In Pandas</v>
       </c>
       <c r="L35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/advanced/22-pandas.html</v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" si="12"/>
         <v>22. &lt;a href="advanced/22-pandas.html"&gt;Working With Data In Pandas&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -2592,33 +2852,33 @@
         <v>146</v>
       </c>
       <c r="C36" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
       <c r="D36" t="s">
         <v>16</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 23. Working With JSON</v>
       </c>
       <c r="F36" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H36" s="8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>23-json</v>
       </c>
       <c r="I36" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>23-json.ipynb</v>
       </c>
       <c r="J36" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>23-json.html</v>
       </c>
       <c r="K36" t="str">
@@ -2626,11 +2886,15 @@
         <v>Lesson 23 Working With JSON</v>
       </c>
       <c r="L36" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/advanced/23-json.html</v>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" si="12"/>
         <v>23. &lt;a href="advanced/23-json.html"&gt;Working With JSON&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -2638,33 +2902,33 @@
         <v>146</v>
       </c>
       <c r="C37" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>24</v>
       </c>
       <c r="D37" t="s">
         <v>46</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 24. Making File Request Over HTTP And FTP</v>
       </c>
       <c r="F37" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>72</v>
       </c>
       <c r="H37" s="8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>24-requesting-files-with-http-ftp</v>
       </c>
       <c r="I37" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>24-requesting-files-with-http-ftp.ipynb</v>
       </c>
       <c r="J37" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>24-requesting-files-with-http-ftp.html</v>
       </c>
       <c r="K37" t="str">
@@ -2672,11 +2936,15 @@
         <v>Lesson 24 Making File Request Over HTTP And FTP</v>
       </c>
       <c r="L37" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/advanced/24-requesting-files-with-http-ftp.html</v>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" si="12"/>
         <v>24. &lt;a href="advanced/24-requesting-files-with-http-ftp.html"&gt;Making File Request Over HTTP And FTP&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -2684,33 +2952,33 @@
         <v>146</v>
       </c>
       <c r="C38" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>25</v>
       </c>
       <c r="D38" t="s">
         <v>17</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 25. Interacting With Databases</v>
       </c>
       <c r="F38" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>73</v>
       </c>
       <c r="H38" s="8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>25-databases</v>
       </c>
       <c r="I38" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>25-databases.ipynb</v>
       </c>
       <c r="J38" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>25-databases.html</v>
       </c>
       <c r="K38" t="str">
@@ -2718,11 +2986,15 @@
         <v>Lesson 25 Interacting With Databases</v>
       </c>
       <c r="L38" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/advanced/25-databases.html</v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" si="12"/>
         <v>25. &lt;a href="advanced/25-databases.html"&gt;Interacting With Databases&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -2730,33 +3002,33 @@
         <v>146</v>
       </c>
       <c r="C39" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>26</v>
       </c>
       <c r="D39" t="s">
         <v>77</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 26. Saving Objects With Pickle</v>
       </c>
       <c r="F39" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>78</v>
       </c>
       <c r="H39" s="8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>26-saving-objects-with-pickle</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>26-saving-objects-with-pickle.ipynb</v>
       </c>
       <c r="J39" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>26-saving-objects-with-pickle.html</v>
       </c>
       <c r="K39" t="str">
@@ -2764,11 +3036,15 @@
         <v>Lesson 26 Saving Objects With Pickle</v>
       </c>
       <c r="L39" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/advanced/26-saving-objects-with-pickle.html</v>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" si="12"/>
         <v>26. &lt;a href="advanced/26-saving-objects-with-pickle.html"&gt;Saving Objects With Pickle&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2776,33 +3052,33 @@
         <v>146</v>
       </c>
       <c r="C40" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>27</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Lesson 27. Error Handling</v>
       </c>
       <c r="F40" s="6">
-        <f t="shared" ref="F40:F51" si="21">IF(C40&lt;10,"0"&amp;C40,C40)</f>
+        <f t="shared" ref="F40:F51" si="22">IF(C40&lt;10,"0"&amp;C40,C40)</f>
         <v>27</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>84</v>
       </c>
       <c r="H40" s="8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>27-error-handling</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>27-error-handling.ipynb</v>
       </c>
       <c r="J40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>27-error-handling.html</v>
       </c>
       <c r="K40" t="str">
@@ -2810,11 +3086,15 @@
         <v>Lesson 27 Error Handling</v>
       </c>
       <c r="L40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/advanced/27-error-handling.html</v>
+      </c>
+      <c r="M40" t="str">
+        <f t="shared" si="12"/>
         <v>27. &lt;a href="advanced/27-error-handling.html"&gt;Error Handling&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -2822,7 +3102,7 @@
         <v>146</v>
       </c>
       <c r="C41" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>28</v>
       </c>
       <c r="D41" t="s">
@@ -2833,7 +3113,7 @@
         <v>Lesson 28. Bringing It All Together</v>
       </c>
       <c r="F41" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>28</v>
       </c>
       <c r="G41" s="6" t="s">
@@ -2856,11 +3136,15 @@
         <v>Lesson 28 Bringing It All Together</v>
       </c>
       <c r="L41" t="str">
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/advanced/28-bringing-it-all-together.html</v>
+      </c>
+      <c r="M41" t="str">
         <f>C41&amp;". &lt;a href="""&amp;A41&amp;"/"&amp;J41&amp;"""&gt;"&amp;D41&amp;"&lt;/a&gt;"</f>
         <v>28. &lt;a href="advanced/28-bringing-it-all-together.html"&gt;Bringing It All Together&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -2868,33 +3152,33 @@
         <v>146</v>
       </c>
       <c r="C42" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29</v>
       </c>
       <c r="D42" t="s">
         <v>93</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" ref="E42:E51" si="22">"Lesson"&amp;" "&amp;C42&amp;"."&amp;" "&amp;D42</f>
+        <f t="shared" ref="E42:E51" si="23">"Lesson"&amp;" "&amp;C42&amp;"."&amp;" "&amp;D42</f>
         <v>Lesson 29. Download A Zip File Over HTTP</v>
       </c>
       <c r="F42" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>29</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>88</v>
       </c>
       <c r="H42" s="8" t="str">
-        <f t="shared" ref="H42:H45" si="23">F42&amp;"-"&amp;G42</f>
+        <f t="shared" ref="H42:H45" si="24">F42&amp;"-"&amp;G42</f>
         <v>29-download-a-zip-file</v>
       </c>
       <c r="I42" t="str">
-        <f t="shared" ref="I42:I45" si="24">F42&amp;"-"&amp;G42&amp;".ipynb"</f>
+        <f t="shared" ref="I42:I45" si="25">F42&amp;"-"&amp;G42&amp;".ipynb"</f>
         <v>29-download-a-zip-file.ipynb</v>
       </c>
       <c r="J42" t="str">
-        <f t="shared" ref="J42:J45" si="25">F42&amp;"-"&amp;G42&amp;".html"</f>
+        <f t="shared" ref="J42:J45" si="26">F42&amp;"-"&amp;G42&amp;".html"</f>
         <v>29-download-a-zip-file.html</v>
       </c>
       <c r="K42" t="str">
@@ -2902,11 +3186,15 @@
         <v>Lesson 29 Download A Zip File Over HTTP</v>
       </c>
       <c r="L42" t="str">
-        <f t="shared" ref="L42:L45" si="26">C42&amp;". &lt;a href="""&amp;A42&amp;"/"&amp;J42&amp;"""&gt;"&amp;D42&amp;"&lt;/a&gt;"</f>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/solutions/29-download-a-zip-file.html</v>
+      </c>
+      <c r="M42" t="str">
+        <f t="shared" ref="M42:M45" si="27">C42&amp;". &lt;a href="""&amp;A42&amp;"/"&amp;J42&amp;"""&gt;"&amp;D42&amp;"&lt;/a&gt;"</f>
         <v>29. &lt;a href="solutions/29-download-a-zip-file.html"&gt;Download A Zip File Over HTTP&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -2914,33 +3202,33 @@
         <v>146</v>
       </c>
       <c r="C43" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
       <c r="D43" t="s">
         <v>54</v>
       </c>
       <c r="E43" t="str">
+        <f t="shared" si="23"/>
+        <v>Lesson 30. Looping Over Files In A Directory</v>
+      </c>
+      <c r="F43" s="6">
         <f t="shared" si="22"/>
-        <v>Lesson 30. Looping Over Files In A Directory</v>
-      </c>
-      <c r="F43" s="6">
-        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>81</v>
       </c>
       <c r="H43" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>30-looping-over-files-in-a-directory</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>30-looping-over-files-in-a-directory.ipynb</v>
       </c>
       <c r="J43" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>30-looping-over-files-in-a-directory.html</v>
       </c>
       <c r="K43" t="str">
@@ -2948,11 +3236,15 @@
         <v>Lesson 30 Looping Over Files In A Directory</v>
       </c>
       <c r="L43" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/solutions/30-looping-over-files-in-a-directory.html</v>
+      </c>
+      <c r="M43" t="str">
+        <f t="shared" si="27"/>
         <v>30. &lt;a href="solutions/30-looping-over-files-in-a-directory.html"&gt;Looping Over Files In A Directory&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>40</v>
       </c>
@@ -2960,33 +3252,33 @@
         <v>146</v>
       </c>
       <c r="C44" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>31</v>
       </c>
       <c r="D44" t="s">
         <v>94</v>
       </c>
       <c r="E44" t="str">
+        <f t="shared" si="23"/>
+        <v>Lesson 31. Convert Comma Delmited Files To Pipe Delimited</v>
+      </c>
+      <c r="F44" s="6">
         <f t="shared" si="22"/>
-        <v>Lesson 31. Convert Comma Delmited Files To Pipe Delimited</v>
-      </c>
-      <c r="F44" s="6">
-        <f t="shared" si="21"/>
         <v>31</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>95</v>
       </c>
       <c r="H44" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>31-convert-file-to-pipe-delimited</v>
       </c>
       <c r="I44" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>31-convert-file-to-pipe-delimited.ipynb</v>
       </c>
       <c r="J44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>31-convert-file-to-pipe-delimited.html</v>
       </c>
       <c r="K44" t="str">
@@ -2994,11 +3286,15 @@
         <v>Lesson 31 Convert Comma Delmited Files To Pipe Delimited</v>
       </c>
       <c r="L44" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/solutions/31-convert-file-to-pipe-delimited.html</v>
+      </c>
+      <c r="M44" t="str">
+        <f t="shared" si="27"/>
         <v>31. &lt;a href="solutions/31-convert-file-to-pipe-delimited.html"&gt;Convert Comma Delmited Files To Pipe Delimited&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>40</v>
       </c>
@@ -3006,33 +3302,33 @@
         <v>146</v>
       </c>
       <c r="C45" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>32</v>
       </c>
       <c r="D45" t="s">
         <v>82</v>
       </c>
       <c r="E45" t="str">
+        <f t="shared" si="23"/>
+        <v>Lesson 32. Combining Multiple CSVs Into One File</v>
+      </c>
+      <c r="F45" s="6">
         <f t="shared" si="22"/>
-        <v>Lesson 32. Combining Multiple CSVs Into One File</v>
-      </c>
-      <c r="F45" s="6">
-        <f t="shared" si="21"/>
         <v>32</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>91</v>
       </c>
       <c r="H45" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>32-combine-csvs-into-one-file</v>
       </c>
       <c r="I45" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>32-combine-csvs-into-one-file.ipynb</v>
       </c>
       <c r="J45" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>32-combine-csvs-into-one-file.html</v>
       </c>
       <c r="K45" t="str">
@@ -3040,11 +3336,15 @@
         <v>Lesson 32 Combining Multiple CSVs Into One File</v>
       </c>
       <c r="L45" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/solutions/32-combine-csvs-into-one-file.html</v>
+      </c>
+      <c r="M45" t="str">
+        <f t="shared" si="27"/>
         <v>32. &lt;a href="solutions/32-combine-csvs-into-one-file.html"&gt;Combining Multiple CSVs Into One File&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -3052,7 +3352,7 @@
         <v>146</v>
       </c>
       <c r="C46" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>33</v>
       </c>
       <c r="D46" t="s">
@@ -3063,7 +3363,7 @@
         <v>Lesson 33. Load Large CSVs Into Data Warehouse Staging Tables</v>
       </c>
       <c r="F46" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>33</v>
       </c>
       <c r="G46" s="6" t="s">
@@ -3086,11 +3386,15 @@
         <v>Lesson 33 Load Large CSVs Into Data Warehouse Staging Tables</v>
       </c>
       <c r="L46" t="str">
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/solutions/33-load-large-csvs-into-data-warehouse.html</v>
+      </c>
+      <c r="M46" t="str">
         <f>C46&amp;". &lt;a href="""&amp;A46&amp;"/"&amp;J46&amp;"""&gt;"&amp;D46&amp;"&lt;/a&gt;"</f>
         <v>33. &lt;a href="solutions/33-load-large-csvs-into-data-warehouse.html"&gt;Load Large CSVs Into Data Warehouse Staging Tables&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -3098,33 +3402,33 @@
         <v>146</v>
       </c>
       <c r="C47" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>34</v>
       </c>
       <c r="D47" s="11" t="s">
         <v>97</v>
       </c>
       <c r="E47" t="str">
+        <f t="shared" si="23"/>
+        <v>Lesson 34. Efficiently Write Large Database Query Results To Disk</v>
+      </c>
+      <c r="F47" s="6">
         <f t="shared" si="22"/>
-        <v>Lesson 34. Efficiently Write Large Database Query Results To Disk</v>
-      </c>
-      <c r="F47" s="6">
-        <f t="shared" si="21"/>
         <v>34</v>
       </c>
       <c r="G47" s="11" t="s">
         <v>96</v>
       </c>
       <c r="H47" s="8" t="str">
-        <f t="shared" ref="H47:H51" si="27">F47&amp;"-"&amp;G47</f>
+        <f t="shared" ref="H47:H51" si="28">F47&amp;"-"&amp;G47</f>
         <v>34-efficient-disk-write</v>
       </c>
       <c r="I47" t="str">
-        <f t="shared" ref="I47:I51" si="28">F47&amp;"-"&amp;G47&amp;".ipynb"</f>
+        <f t="shared" ref="I47:I51" si="29">F47&amp;"-"&amp;G47&amp;".ipynb"</f>
         <v>34-efficient-disk-write.ipynb</v>
       </c>
       <c r="J47" t="str">
-        <f t="shared" ref="J47:J51" si="29">F47&amp;"-"&amp;G47&amp;".html"</f>
+        <f t="shared" ref="J47:J51" si="30">F47&amp;"-"&amp;G47&amp;".html"</f>
         <v>34-efficient-disk-write.html</v>
       </c>
       <c r="K47" t="str">
@@ -3132,11 +3436,15 @@
         <v>Lesson 34 Efficiently Write Large Database Query Results To Disk</v>
       </c>
       <c r="L47" t="str">
-        <f t="shared" ref="L47:L50" si="30">C47&amp;". &lt;a href="""&amp;A47&amp;"/"&amp;J47&amp;"""&gt;"&amp;D47&amp;"&lt;/a&gt;"</f>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/solutions/34-efficient-disk-write.html</v>
+      </c>
+      <c r="M47" t="str">
+        <f t="shared" ref="M47:M50" si="31">C47&amp;". &lt;a href="""&amp;A47&amp;"/"&amp;J47&amp;"""&gt;"&amp;D47&amp;"&lt;/a&gt;"</f>
         <v>34. &lt;a href="solutions/34-efficient-disk-write.html"&gt;Efficiently Write Large Database Query Results To Disk&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>40</v>
       </c>
@@ -3144,33 +3452,33 @@
         <v>146</v>
       </c>
       <c r="C48" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>35</v>
       </c>
       <c r="D48" s="11" t="s">
         <v>137</v>
       </c>
       <c r="E48" t="str">
+        <f t="shared" si="23"/>
+        <v>Lesson 35. Working With SFTP In The Real World</v>
+      </c>
+      <c r="F48" s="6">
         <f t="shared" si="22"/>
-        <v>Lesson 35. Working With SFTP In The Real World</v>
-      </c>
-      <c r="F48" s="6">
-        <f t="shared" si="21"/>
         <v>35</v>
       </c>
       <c r="G48" s="11" t="s">
         <v>139</v>
       </c>
       <c r="H48" s="8" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>35-sftp-in-the-real-world</v>
       </c>
       <c r="I48" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>35-sftp-in-the-real-world.ipynb</v>
       </c>
       <c r="J48" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>35-sftp-in-the-real-world.html</v>
       </c>
       <c r="K48" t="str">
@@ -3178,11 +3486,15 @@
         <v>Lesson 35 Working With SFTP In The Real World</v>
       </c>
       <c r="L48" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/solutions/35-sftp-in-the-real-world.html</v>
+      </c>
+      <c r="M48" t="str">
+        <f t="shared" si="31"/>
         <v>35. &lt;a href="solutions/35-sftp-in-the-real-world.html"&gt;Working With SFTP In The Real World&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>40</v>
       </c>
@@ -3190,33 +3502,33 @@
         <v>146</v>
       </c>
       <c r="C49" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>36</v>
       </c>
       <c r="D49" t="s">
         <v>138</v>
       </c>
       <c r="E49" t="str">
+        <f t="shared" si="23"/>
+        <v>Lesson 36. Executing Python From SQL Server Agent</v>
+      </c>
+      <c r="F49" s="6">
         <f t="shared" si="22"/>
-        <v>Lesson 36. Executing Python From SQL Server Agent</v>
-      </c>
-      <c r="F49" s="6">
-        <f t="shared" si="21"/>
         <v>36</v>
       </c>
       <c r="G49" s="11" t="s">
         <v>140</v>
       </c>
       <c r="H49" s="8" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>36-run-python-from-sql-server</v>
       </c>
       <c r="I49" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>36-run-python-from-sql-server.ipynb</v>
       </c>
       <c r="J49" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>36-run-python-from-sql-server.html</v>
       </c>
       <c r="K49" t="str">
@@ -3224,11 +3536,15 @@
         <v>Lesson 36 Executing Python From SQL Server Agent</v>
       </c>
       <c r="L49" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/solutions/36-run-python-from-sql-server.html</v>
+      </c>
+      <c r="M49" t="str">
+        <f t="shared" si="31"/>
         <v>36. &lt;a href="solutions/36-run-python-from-sql-server.html"&gt;Executing Python From SQL Server Agent&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -3236,33 +3552,33 @@
         <v>146</v>
       </c>
       <c r="C50" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>37</v>
       </c>
       <c r="D50" t="s">
         <v>100</v>
       </c>
       <c r="E50" t="str">
+        <f t="shared" si="23"/>
+        <v>Lesson 37. Final Project</v>
+      </c>
+      <c r="F50" s="6">
         <f t="shared" si="22"/>
-        <v>Lesson 37. Final Project</v>
-      </c>
-      <c r="F50" s="6">
-        <f t="shared" si="21"/>
         <v>37</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>101</v>
       </c>
       <c r="H50" s="5" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>37-final-project</v>
       </c>
       <c r="I50" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>37-final-project.ipynb</v>
       </c>
       <c r="J50" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>37-final-project.html</v>
       </c>
       <c r="K50" t="str">
@@ -3270,11 +3586,15 @@
         <v>Lesson 37 Final Project</v>
       </c>
       <c r="L50" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/project/37-final-project.html</v>
+      </c>
+      <c r="M50" t="str">
+        <f t="shared" si="31"/>
         <v>37. &lt;a href="project/37-final-project.html"&gt;Final Project&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>98</v>
       </c>
@@ -3282,33 +3602,33 @@
         <v>146</v>
       </c>
       <c r="C51" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>38</v>
       </c>
       <c r="D51" t="s">
         <v>104</v>
       </c>
       <c r="E51" t="str">
+        <f t="shared" si="23"/>
+        <v>Lesson 38. Further Training</v>
+      </c>
+      <c r="F51" s="6">
         <f t="shared" si="22"/>
-        <v>Lesson 38. Further Training</v>
-      </c>
-      <c r="F51" s="6">
-        <f t="shared" si="21"/>
         <v>38</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>105</v>
       </c>
       <c r="H51" s="5" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>38-further-training</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>38-further-training.ipynb</v>
       </c>
       <c r="J51" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>38-further-training.html</v>
       </c>
       <c r="K51" t="str">
@@ -3316,12 +3636,16 @@
         <v>Lesson 38 Further Training</v>
       </c>
       <c r="L51" t="str">
+        <f t="shared" si="6"/>
+        <v>https://learn.massstreet.net/python/project/38-further-training.html</v>
+      </c>
+      <c r="M51" t="str">
         <f>C51&amp;". &lt;a href="""&amp;A51&amp;"/"&amp;J51&amp;"""&gt;"&amp;D51&amp;"&lt;/a&gt;"</f>
         <v>38. &lt;a href="project/38-further-training.html"&gt;Further Training&lt;/a&gt;</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L51" xr:uid="{C26BCB42-6FAD-4781-AC88-8DB659BD4328}"/>
+  <autoFilter ref="A1:M51" xr:uid="{C26BCB42-6FAD-4781-AC88-8DB659BD4328}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -3349,8 +3673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA4136B-2C83-4DC0-A4CA-D1A27C680A6D}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3644,11 +3968,11 @@
         <v>174</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" ref="D3:D66" si="2">B14&amp;" "&amp;"With Python"</f>
+        <f t="shared" ref="D14:D49" si="2">B14&amp;" "&amp;"With Python"</f>
         <v>Lesson 1. Obligatory Hello World With Python</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" ref="E3:E66" si="3">"In this lesson,"&amp;" "&amp;C14</f>
+        <f t="shared" ref="E14:E49" si="3">"In this lesson,"&amp;" "&amp;C14</f>
         <v>In this lesson, I offer the standard Hello World lesson that is required of every code tutorial on planet Earth.</v>
       </c>
     </row>
@@ -3682,13 +4006,16 @@
         <f>'Lesson File Xref'!E16</f>
         <v>Lesson 3. Data Types</v>
       </c>
+      <c r="C16" s="11" t="s">
+        <v>176</v>
+      </c>
       <c r="D16" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 3. Data Types With Python</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, I teach you the different kinds of data types in Python!</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3700,13 +4027,16 @@
         <f>'Lesson File Xref'!E17</f>
         <v>Lesson 4. Variables</v>
       </c>
+      <c r="C17" s="11" t="s">
+        <v>177</v>
+      </c>
       <c r="D17" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 4. Variables With Python</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, I teach you how to work with variables!</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3718,13 +4048,16 @@
         <f>'Lesson File Xref'!E18</f>
         <v>Lesson 5. String Concatenation</v>
       </c>
+      <c r="C18" s="11" t="s">
+        <v>178</v>
+      </c>
       <c r="D18" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 5. String Concatenation With Python</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, I teach you how to smoosh stuff together!</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3736,13 +4069,16 @@
         <f>'Lesson File Xref'!E19</f>
         <v>Lesson 6. Arithmetic Operators</v>
       </c>
+      <c r="C19" s="11" t="s">
+        <v>179</v>
+      </c>
       <c r="D19" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 6. Arithmetic Operators With Python</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, I teach you how to do third grade math with code!</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3754,13 +4090,16 @@
         <f>'Lesson File Xref'!E20</f>
         <v>Lesson 7. Making Decisions</v>
       </c>
+      <c r="C20" s="11" t="s">
+        <v>180</v>
+      </c>
       <c r="D20" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 7. Making Decisions With Python</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, I'm going to show you the 10 different methods to make decisions with code!</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3772,13 +4111,16 @@
         <f>'Lesson File Xref'!E21</f>
         <v>Lesson 8. Control Flow With if-elif-else</v>
       </c>
+      <c r="C21" s="11" t="s">
+        <v>181</v>
+      </c>
       <c r="D21" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 8. Control Flow With if-elif-else With Python</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, I teach you how to control your roll!</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3790,13 +4132,16 @@
         <f>'Lesson File Xref'!E22</f>
         <v>Lesson 9. Control Flow With While</v>
       </c>
+      <c r="C22" s="11" t="s">
+        <v>182</v>
+      </c>
       <c r="D22" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 9. Control Flow With While With Python</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, we talk about talk about controlling flow again but this time, it's gonna take a while!</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3808,13 +4153,16 @@
         <f>'Lesson File Xref'!E23</f>
         <v>Lesson 10. Data Structures Part I: List</v>
       </c>
+      <c r="C23" s="11" t="s">
+        <v>183</v>
+      </c>
       <c r="D23" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 10. Data Structures Part I: List With Python</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, we talk about list!</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3826,13 +4174,16 @@
         <f>'Lesson File Xref'!E24</f>
         <v>Lesson 11. Data Structures Part II: Tuples</v>
       </c>
+      <c r="C24" s="11" t="s">
+        <v>184</v>
+      </c>
       <c r="D24" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 11. Data Structures Part II: Tuples With Python</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, we talk about tuples!</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3844,13 +4195,16 @@
         <f>'Lesson File Xref'!E25</f>
         <v>Lesson 12. Data Structures Part III: Dictionaries</v>
       </c>
+      <c r="C25" s="11" t="s">
+        <v>185</v>
+      </c>
       <c r="D25" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 12. Data Structures Part III: Dictionaries With Python</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, we talk about dictionaries!</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3862,13 +4216,16 @@
         <f>'Lesson File Xref'!E26</f>
         <v>Lesson 13. Looping With for</v>
       </c>
+      <c r="C26" s="11" t="s">
+        <v>186</v>
+      </c>
       <c r="D26" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 13. Looping With for With Python</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, we get loopy!</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3880,13 +4237,16 @@
         <f>'Lesson File Xref'!E27</f>
         <v>Lesson 14. Functions</v>
       </c>
+      <c r="C27" s="11" t="s">
+        <v>187</v>
+      </c>
       <c r="D27" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 14. Functions With Python</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, we out here trying to function!</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3898,13 +4258,16 @@
         <f>'Lesson File Xref'!E28</f>
         <v>Lesson 15. Importing Modules</v>
       </c>
+      <c r="C28" s="11" t="s">
+        <v>188</v>
+      </c>
       <c r="D28" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 15. Importing Modules With Python</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, I show you the true power of Python. Importing Modules!</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3916,13 +4279,16 @@
         <f>'Lesson File Xref'!E29</f>
         <v>Lesson 16. Python Programming Standards</v>
       </c>
+      <c r="C29" s="11" t="s">
+        <v>189</v>
+      </c>
       <c r="D29" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 16. Python Programming Standards With Python</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, we grow some self respect and get some standards as software engineers!</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3934,13 +4300,16 @@
         <f>'Lesson File Xref'!E30</f>
         <v>Lesson 17. Functional Programing With map</v>
       </c>
+      <c r="C30" s="11" t="s">
+        <v>190</v>
+      </c>
       <c r="D30" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 17. Functional Programing With map With Python</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, we explore the alternative paradigm to object oriented programming. Functional programming!</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3952,13 +4321,16 @@
         <f>'Lesson File Xref'!E31</f>
         <v>Lesson 18. Generators</v>
       </c>
+      <c r="C31" s="11" t="s">
+        <v>191</v>
+      </c>
       <c r="D31" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 18. Generators With Python</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, we'll be generating some discussion about generators!</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3970,13 +4342,16 @@
         <f>'Lesson File Xref'!E32</f>
         <v>Lesson 19. Comprehensions</v>
       </c>
+      <c r="C32" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="D32" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 19. Comprehensions With Python</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, you're going to understand the words that are coming out of my mouth! (Comprehension. Get it?)</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3988,13 +4363,16 @@
         <f>'Lesson File Xref'!E33</f>
         <v>Lesson 20. Basic File Operations</v>
       </c>
+      <c r="C33" s="11" t="s">
+        <v>193</v>
+      </c>
       <c r="D33" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 20. Basic File Operations With Python</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, it's ok to be basic because we're going to talk about how to work with files.</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -4006,13 +4384,16 @@
         <f>'Lesson File Xref'!E34</f>
         <v>Lesson 21. Working With Data In NumPy</v>
       </c>
+      <c r="C34" s="11" t="s">
+        <v>194</v>
+      </c>
       <c r="D34" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 21. Working With Data In NumPy With Python</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, I'll give you an intro to Pandas's less attractive cousin.</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -4024,13 +4405,16 @@
         <f>'Lesson File Xref'!E35</f>
         <v>Lesson 22. Working With Data In Pandas</v>
       </c>
+      <c r="C35" s="11" t="s">
+        <v>195</v>
+      </c>
       <c r="D35" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 22. Working With Data In Pandas With Python</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, you'll be sad to discover that you won't be working with cute bears.</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -4042,13 +4426,16 @@
         <f>'Lesson File Xref'!E36</f>
         <v>Lesson 23. Working With JSON</v>
       </c>
+      <c r="C36" s="11" t="s">
+        <v>196</v>
+      </c>
       <c r="D36" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 23. Working With JSON With Python</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, you'll learn why JSON is everything XML was SUPPOSED to be.</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -4060,13 +4447,16 @@
         <f>'Lesson File Xref'!E37</f>
         <v>Lesson 24. Making File Request Over HTTP And FTP</v>
       </c>
+      <c r="C37" s="11" t="s">
+        <v>197</v>
+      </c>
       <c r="D37" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 24. Making File Request Over HTTP And FTP With Python</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, we'll learn how to transfer files with various internet protocols.</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -4078,13 +4468,16 @@
         <f>'Lesson File Xref'!E38</f>
         <v>Lesson 25. Interacting With Databases</v>
       </c>
+      <c r="C38" s="11" t="s">
+        <v>198</v>
+      </c>
       <c r="D38" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 25. Interacting With Databases With Python</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, we're gonna be all "SELECT * FROM" as we learn to get data from databases!</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -4096,13 +4489,16 @@
         <f>'Lesson File Xref'!E39</f>
         <v>Lesson 26. Saving Objects With Pickle</v>
       </c>
+      <c r="C39" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="D39" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 26. Saving Objects With Pickle With Python</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, you're going to blow your grandma's mind when you tell her you learned how to pickle something!</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -4114,13 +4510,16 @@
         <f>'Lesson File Xref'!E40</f>
         <v>Lesson 27. Error Handling</v>
       </c>
+      <c r="C40" s="11" t="s">
+        <v>200</v>
+      </c>
       <c r="D40" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 27. Error Handling With Python</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, I teach you how to deal with the crazy things users like to do to your code.</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -4132,13 +4531,16 @@
         <f>'Lesson File Xref'!E41</f>
         <v>Lesson 28. Bringing It All Together</v>
       </c>
+      <c r="C41" s="11" t="s">
+        <v>201</v>
+      </c>
       <c r="D41" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 28. Bringing It All Together With Python</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, we're going to integrate all of the concepts we spoke about into a single concept.</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -4150,13 +4552,16 @@
         <f>'Lesson File Xref'!E42</f>
         <v>Lesson 29. Download A Zip File Over HTTP</v>
       </c>
+      <c r="C42" s="11" t="s">
+        <v>202</v>
+      </c>
       <c r="D42" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 29. Download A Zip File Over HTTP With Python</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, we get into tips, tricks, and tactics. This is how I get zip files over the internet. It's harder than you think!</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -4168,13 +4573,16 @@
         <f>'Lesson File Xref'!E43</f>
         <v>Lesson 30. Looping Over Files In A Directory</v>
       </c>
+      <c r="C43" s="11" t="s">
+        <v>207</v>
+      </c>
       <c r="D43" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 30. Looping Over Files In A Directory With Python</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, you finally get to see why building ETL with SSIS packages is dumb. I mean, there is just no other word for it.</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -4186,13 +4594,16 @@
         <f>'Lesson File Xref'!E44</f>
         <v>Lesson 31. Convert Comma Delmited Files To Pipe Delimited</v>
       </c>
+      <c r="C44" s="11" t="s">
+        <v>203</v>
+      </c>
       <c r="D44" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 31. Convert Comma Delmited Files To Pipe Delimited With Python</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, you'll learn a better file delimiter than the comma.</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -4204,13 +4615,16 @@
         <f>'Lesson File Xref'!E45</f>
         <v>Lesson 32. Combining Multiple CSVs Into One File</v>
       </c>
+      <c r="C45" s="11" t="s">
+        <v>204</v>
+      </c>
       <c r="D45" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 32. Combining Multiple CSVs Into One File With Python</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, I teach you how to take a bunch of little files and make one big file which comes in handy when loading database tables.</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -4222,13 +4636,16 @@
         <f>'Lesson File Xref'!E46</f>
         <v>Lesson 33. Load Large CSVs Into Data Warehouse Staging Tables</v>
       </c>
+      <c r="C46" s="11" t="s">
+        <v>208</v>
+      </c>
       <c r="D46" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 33. Load Large CSVs Into Data Warehouse Staging Tables With Python</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, I teach you another highly efficient method of loading flat files into tables.</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -4240,13 +4657,16 @@
         <f>'Lesson File Xref'!E47</f>
         <v>Lesson 34. Efficiently Write Large Database Query Results To Disk</v>
       </c>
+      <c r="C47" s="11" t="s">
+        <v>205</v>
+      </c>
       <c r="D47" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 34. Efficiently Write Large Database Query Results To Disk With Python</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, I teach you how to write a large file to disk quickly!</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -4276,13 +4696,16 @@
         <f>'Lesson File Xref'!E49</f>
         <v>Lesson 36. Executing Python From SQL Server Agent</v>
       </c>
+      <c r="C49" s="11" t="s">
+        <v>206</v>
+      </c>
       <c r="D49" t="str">
         <f t="shared" si="2"/>
         <v>Lesson 36. Executing Python From SQL Server Agent With Python</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">In this lesson, </v>
+        <v>In this lesson, I teach you how to use PowerShell to run your Python scripts from SQL Server.</v>
       </c>
     </row>
   </sheetData>
@@ -4292,12 +4715,1211 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278C3861-DE5D-4C87-8987-7B291EC247BE}">
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="82.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="117.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="86" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="207" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>'Lesson File Xref'!A14</f>
+        <v>basics</v>
+      </c>
+      <c r="B2" s="16">
+        <f>'Lesson File Xref'!C14</f>
+        <v>1</v>
+      </c>
+      <c r="C2" t="str">
+        <f>LOWER('Lesson File Xref'!D14)</f>
+        <v>obligatory hello world</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"Here is your daily #Python lesson! Today in lesson "&amp;B2&amp;" we're going to talk about the inevitable"</f>
+        <v>Here is your daily #Python lesson! Today in lesson 1 we're going to talk about the inevitable</v>
+      </c>
+      <c r="E2" t="str">
+        <f>D2&amp;" "&amp;C2&amp;"."</f>
+        <v>Here is your daily #Python lesson! Today in lesson 1 we're going to talk about the inevitable obligatory hello world.</v>
+      </c>
+      <c r="F2" t="str">
+        <f>'Lesson File Xref'!L14</f>
+        <v>https://learn.massstreet.net/python/basics/01-hello-world.html</v>
+      </c>
+      <c r="G2" t="str">
+        <f>E2&amp;CHAR(10)&amp;CHAR(10)&amp;F2&amp;CHAR(10)</f>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 1 we're going to talk about the inevitable obligatory hello world.
+https://learn.massstreet.net/python/basics/01-hello-world.html
+</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>'Lesson File Xref'!A15</f>
+        <v>basics</v>
+      </c>
+      <c r="B3" s="16">
+        <f>'Lesson File Xref'!C15</f>
+        <v>2</v>
+      </c>
+      <c r="C3" t="str">
+        <f>LOWER('Lesson File Xref'!D15)</f>
+        <v>code comments</v>
+      </c>
+      <c r="D3" t="str">
+        <f>"Here is your daily #Python lesson! Today in lesson "&amp;B3&amp;" we're going to talk about"</f>
+        <v>Here is your daily #Python lesson! Today in lesson 2 we're going to talk about</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E37" si="0">D3&amp;" "&amp;C3&amp;"."</f>
+        <v>Here is your daily #Python lesson! Today in lesson 2 we're going to talk about code comments.</v>
+      </c>
+      <c r="F3" t="str">
+        <f>'Lesson File Xref'!L15</f>
+        <v>https://learn.massstreet.net/python/basics/02-code-comments.html</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G37" si="1">E3&amp;CHAR(10)&amp;CHAR(10)&amp;F3&amp;CHAR(10)</f>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 2 we're going to talk about code comments.
+https://learn.massstreet.net/python/basics/02-code-comments.html
+</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>'Lesson File Xref'!A16</f>
+        <v>basics</v>
+      </c>
+      <c r="B4" s="16">
+        <f>'Lesson File Xref'!C16</f>
+        <v>3</v>
+      </c>
+      <c r="C4" t="str">
+        <f>LOWER('Lesson File Xref'!D16)</f>
+        <v>data types</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D37" si="2">"Here is your daily #Python lesson! Today in lesson "&amp;B4&amp;" we're going to talk about"</f>
+        <v>Here is your daily #Python lesson! Today in lesson 3 we're going to talk about</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 3 we're going to talk about data types.</v>
+      </c>
+      <c r="F4" t="str">
+        <f>'Lesson File Xref'!L16</f>
+        <v>https://learn.massstreet.net/python/basics/03-data-types.html</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 3 we're going to talk about data types.
+https://learn.massstreet.net/python/basics/03-data-types.html
+</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>'Lesson File Xref'!A17</f>
+        <v>basics</v>
+      </c>
+      <c r="B5" s="16">
+        <f>'Lesson File Xref'!C17</f>
+        <v>4</v>
+      </c>
+      <c r="C5" t="str">
+        <f>LOWER('Lesson File Xref'!D17)</f>
+        <v>variables</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 4 we're going to talk about</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 4 we're going to talk about variables.</v>
+      </c>
+      <c r="F5" t="str">
+        <f>'Lesson File Xref'!L17</f>
+        <v>https://learn.massstreet.net/python/basics/04-variables.html</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 4 we're going to talk about variables.
+https://learn.massstreet.net/python/basics/04-variables.html
+</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>'Lesson File Xref'!A18</f>
+        <v>basics</v>
+      </c>
+      <c r="B6" s="16">
+        <f>'Lesson File Xref'!C18</f>
+        <v>5</v>
+      </c>
+      <c r="C6" t="str">
+        <f>LOWER('Lesson File Xref'!D18)</f>
+        <v>string concatenation</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 5 we're going to talk about</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 5 we're going to talk about string concatenation.</v>
+      </c>
+      <c r="F6" t="str">
+        <f>'Lesson File Xref'!L18</f>
+        <v>https://learn.massstreet.net/python/basics/05-string-concatenation.html</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 5 we're going to talk about string concatenation.
+https://learn.massstreet.net/python/basics/05-string-concatenation.html
+</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>'Lesson File Xref'!A19</f>
+        <v>basics</v>
+      </c>
+      <c r="B7" s="16">
+        <f>'Lesson File Xref'!C19</f>
+        <v>6</v>
+      </c>
+      <c r="C7" t="str">
+        <f>LOWER('Lesson File Xref'!D19)</f>
+        <v>arithmetic operators</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 6 we're going to talk about</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 6 we're going to talk about arithmetic operators.</v>
+      </c>
+      <c r="F7" t="str">
+        <f>'Lesson File Xref'!L19</f>
+        <v>https://learn.massstreet.net/python/basics/06-arithmetic-operators.html</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 6 we're going to talk about arithmetic operators.
+https://learn.massstreet.net/python/basics/06-arithmetic-operators.html
+</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>'Lesson File Xref'!A20</f>
+        <v>basics</v>
+      </c>
+      <c r="B8" s="16">
+        <f>'Lesson File Xref'!C20</f>
+        <v>7</v>
+      </c>
+      <c r="C8" t="str">
+        <f>LOWER('Lesson File Xref'!D20)</f>
+        <v>making decisions</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 7 we're going to talk about</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 7 we're going to talk about making decisions.</v>
+      </c>
+      <c r="F8" t="str">
+        <f>'Lesson File Xref'!L20</f>
+        <v>https://learn.massstreet.net/python/basics/07-making-decisions.html</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 7 we're going to talk about making decisions.
+https://learn.massstreet.net/python/basics/07-making-decisions.html
+</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>'Lesson File Xref'!A21</f>
+        <v>basics</v>
+      </c>
+      <c r="B9" s="16">
+        <f>'Lesson File Xref'!C21</f>
+        <v>8</v>
+      </c>
+      <c r="C9" t="str">
+        <f>LOWER('Lesson File Xref'!D21)</f>
+        <v>control flow with if-elif-else</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 8 we're going to talk about</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 8 we're going to talk about control flow with if-elif-else.</v>
+      </c>
+      <c r="F9" t="str">
+        <f>'Lesson File Xref'!L21</f>
+        <v>https://learn.massstreet.net/python/basics/08-control-flow-if-else.html</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 8 we're going to talk about control flow with if-elif-else.
+https://learn.massstreet.net/python/basics/08-control-flow-if-else.html
+</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>'Lesson File Xref'!A22</f>
+        <v>basics</v>
+      </c>
+      <c r="B10" s="16">
+        <f>'Lesson File Xref'!C22</f>
+        <v>9</v>
+      </c>
+      <c r="C10" t="str">
+        <f>LOWER('Lesson File Xref'!D22)</f>
+        <v>control flow with while</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 9 we're going to talk about</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 9 we're going to talk about control flow with while.</v>
+      </c>
+      <c r="F10" t="str">
+        <f>'Lesson File Xref'!L22</f>
+        <v>https://learn.massstreet.net/python/basics/09-control-flow-while.html</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 9 we're going to talk about control flow with while.
+https://learn.massstreet.net/python/basics/09-control-flow-while.html
+</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>'Lesson File Xref'!A23</f>
+        <v>basics</v>
+      </c>
+      <c r="B11" s="16">
+        <f>'Lesson File Xref'!C23</f>
+        <v>10</v>
+      </c>
+      <c r="C11" t="str">
+        <f>LOWER('Lesson File Xref'!D23)</f>
+        <v>data structures part i: list</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 10 we're going to talk about</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 10 we're going to talk about data structures part i: list.</v>
+      </c>
+      <c r="F11" t="str">
+        <f>'Lesson File Xref'!L23</f>
+        <v>https://learn.massstreet.net/python/basics/10-list.html</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 10 we're going to talk about data structures part i: list.
+https://learn.massstreet.net/python/basics/10-list.html
+</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>'Lesson File Xref'!A24</f>
+        <v>basics</v>
+      </c>
+      <c r="B12" s="16">
+        <f>'Lesson File Xref'!C24</f>
+        <v>11</v>
+      </c>
+      <c r="C12" t="str">
+        <f>LOWER('Lesson File Xref'!D24)</f>
+        <v>data structures part ii: tuples</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 11 we're going to talk about</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 11 we're going to talk about data structures part ii: tuples.</v>
+      </c>
+      <c r="F12" t="str">
+        <f>'Lesson File Xref'!L24</f>
+        <v>https://learn.massstreet.net/python/basics/11-tuples.html</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 11 we're going to talk about data structures part ii: tuples.
+https://learn.massstreet.net/python/basics/11-tuples.html
+</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f>'Lesson File Xref'!A25</f>
+        <v>basics</v>
+      </c>
+      <c r="B13" s="16">
+        <f>'Lesson File Xref'!C25</f>
+        <v>12</v>
+      </c>
+      <c r="C13" t="str">
+        <f>LOWER('Lesson File Xref'!D25)</f>
+        <v>data structures part iii: dictionaries</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 12 we're going to talk about</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 12 we're going to talk about data structures part iii: dictionaries.</v>
+      </c>
+      <c r="F13" t="str">
+        <f>'Lesson File Xref'!L25</f>
+        <v>https://learn.massstreet.net/python/basics/12-dictionaries.html</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 12 we're going to talk about data structures part iii: dictionaries.
+https://learn.massstreet.net/python/basics/12-dictionaries.html
+</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>'Lesson File Xref'!A26</f>
+        <v>basics</v>
+      </c>
+      <c r="B14" s="16">
+        <f>'Lesson File Xref'!C26</f>
+        <v>13</v>
+      </c>
+      <c r="C14" t="str">
+        <f>LOWER('Lesson File Xref'!D26)</f>
+        <v>looping with for</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 13 we're going to talk about</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 13 we're going to talk about looping with for.</v>
+      </c>
+      <c r="F14" t="str">
+        <f>'Lesson File Xref'!L26</f>
+        <v>https://learn.massstreet.net/python/basics/13-looping-with-for.html</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 13 we're going to talk about looping with for.
+https://learn.massstreet.net/python/basics/13-looping-with-for.html
+</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>'Lesson File Xref'!A27</f>
+        <v>basics</v>
+      </c>
+      <c r="B15" s="16">
+        <f>'Lesson File Xref'!C27</f>
+        <v>14</v>
+      </c>
+      <c r="C15" t="str">
+        <f>LOWER('Lesson File Xref'!D27)</f>
+        <v>functions</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 14 we're going to talk about</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 14 we're going to talk about functions.</v>
+      </c>
+      <c r="F15" t="str">
+        <f>'Lesson File Xref'!L27</f>
+        <v>https://learn.massstreet.net/python/basics/14-functions.html</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 14 we're going to talk about functions.
+https://learn.massstreet.net/python/basics/14-functions.html
+</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f>'Lesson File Xref'!A28</f>
+        <v>basics</v>
+      </c>
+      <c r="B16" s="16">
+        <f>'Lesson File Xref'!C28</f>
+        <v>15</v>
+      </c>
+      <c r="C16" t="str">
+        <f>LOWER('Lesson File Xref'!D28)</f>
+        <v>importing modules</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 15 we're going to talk about</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 15 we're going to talk about importing modules.</v>
+      </c>
+      <c r="F16" t="str">
+        <f>'Lesson File Xref'!L28</f>
+        <v>https://learn.massstreet.net/python/basics/15-importing-modules.html</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 15 we're going to talk about importing modules.
+https://learn.massstreet.net/python/basics/15-importing-modules.html
+</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>'Lesson File Xref'!A29</f>
+        <v>basics</v>
+      </c>
+      <c r="B17" s="16">
+        <f>'Lesson File Xref'!C29</f>
+        <v>16</v>
+      </c>
+      <c r="C17" t="str">
+        <f>LOWER('Lesson File Xref'!D29)</f>
+        <v>python programming standards</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 16 we're going to talk about</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 16 we're going to talk about python programming standards.</v>
+      </c>
+      <c r="F17" t="str">
+        <f>'Lesson File Xref'!L29</f>
+        <v>https://learn.massstreet.net/python/basics/16-python-programming-standards.html</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 16 we're going to talk about python programming standards.
+https://learn.massstreet.net/python/basics/16-python-programming-standards.html
+</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>'Lesson File Xref'!A30</f>
+        <v>advanced</v>
+      </c>
+      <c r="B18" s="16">
+        <f>'Lesson File Xref'!C30</f>
+        <v>17</v>
+      </c>
+      <c r="C18" t="str">
+        <f>LOWER('Lesson File Xref'!D30)</f>
+        <v>functional programing with map</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 17 we're going to talk about</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 17 we're going to talk about functional programing with map.</v>
+      </c>
+      <c r="F18" t="str">
+        <f>'Lesson File Xref'!L30</f>
+        <v>https://learn.massstreet.net/python/advanced/17-map.html</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 17 we're going to talk about functional programing with map.
+https://learn.massstreet.net/python/advanced/17-map.html
+</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>'Lesson File Xref'!A31</f>
+        <v>advanced</v>
+      </c>
+      <c r="B19" s="16">
+        <f>'Lesson File Xref'!C31</f>
+        <v>18</v>
+      </c>
+      <c r="C19" t="str">
+        <f>LOWER('Lesson File Xref'!D31)</f>
+        <v>generators</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 18 we're going to talk about</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 18 we're going to talk about generators.</v>
+      </c>
+      <c r="F19" t="str">
+        <f>'Lesson File Xref'!L31</f>
+        <v>https://learn.massstreet.net/python/advanced/18-generators.html</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 18 we're going to talk about generators.
+https://learn.massstreet.net/python/advanced/18-generators.html
+</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>'Lesson File Xref'!A32</f>
+        <v>advanced</v>
+      </c>
+      <c r="B20" s="16">
+        <f>'Lesson File Xref'!C32</f>
+        <v>19</v>
+      </c>
+      <c r="C20" t="str">
+        <f>LOWER('Lesson File Xref'!D32)</f>
+        <v>comprehensions</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 19 we're going to talk about</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 19 we're going to talk about comprehensions.</v>
+      </c>
+      <c r="F20" t="str">
+        <f>'Lesson File Xref'!L32</f>
+        <v>https://learn.massstreet.net/python/advanced/19-comprehensions.html</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 19 we're going to talk about comprehensions.
+https://learn.massstreet.net/python/advanced/19-comprehensions.html
+</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>'Lesson File Xref'!A33</f>
+        <v>advanced</v>
+      </c>
+      <c r="B21" s="16">
+        <f>'Lesson File Xref'!C33</f>
+        <v>20</v>
+      </c>
+      <c r="C21" t="str">
+        <f>LOWER('Lesson File Xref'!D33)</f>
+        <v>basic file operations</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 20 we're going to talk about</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 20 we're going to talk about basic file operations.</v>
+      </c>
+      <c r="F21" t="str">
+        <f>'Lesson File Xref'!L33</f>
+        <v>https://learn.massstreet.net/python/advanced/20-basic-file-operations.html</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 20 we're going to talk about basic file operations.
+https://learn.massstreet.net/python/advanced/20-basic-file-operations.html
+</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f>'Lesson File Xref'!A34</f>
+        <v>advanced</v>
+      </c>
+      <c r="B22" s="16">
+        <f>'Lesson File Xref'!C34</f>
+        <v>21</v>
+      </c>
+      <c r="C22" t="str">
+        <f>LOWER('Lesson File Xref'!D34)</f>
+        <v>working with data in numpy</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 21 we're going to talk about</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 21 we're going to talk about working with data in numpy.</v>
+      </c>
+      <c r="F22" t="str">
+        <f>'Lesson File Xref'!L34</f>
+        <v>https://learn.massstreet.net/python/advanced/21-numpy.html</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 21 we're going to talk about working with data in numpy.
+https://learn.massstreet.net/python/advanced/21-numpy.html
+</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f>'Lesson File Xref'!A35</f>
+        <v>advanced</v>
+      </c>
+      <c r="B23" s="16">
+        <f>'Lesson File Xref'!C35</f>
+        <v>22</v>
+      </c>
+      <c r="C23" t="str">
+        <f>LOWER('Lesson File Xref'!D35)</f>
+        <v>working with data in pandas</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 22 we're going to talk about</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 22 we're going to talk about working with data in pandas.</v>
+      </c>
+      <c r="F23" t="str">
+        <f>'Lesson File Xref'!L35</f>
+        <v>https://learn.massstreet.net/python/advanced/22-pandas.html</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 22 we're going to talk about working with data in pandas.
+https://learn.massstreet.net/python/advanced/22-pandas.html
+</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>'Lesson File Xref'!A36</f>
+        <v>advanced</v>
+      </c>
+      <c r="B24" s="16">
+        <f>'Lesson File Xref'!C36</f>
+        <v>23</v>
+      </c>
+      <c r="C24" t="str">
+        <f>LOWER('Lesson File Xref'!D36)</f>
+        <v>working with json</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 23 we're going to talk about</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 23 we're going to talk about working with json.</v>
+      </c>
+      <c r="F24" t="str">
+        <f>'Lesson File Xref'!L36</f>
+        <v>https://learn.massstreet.net/python/advanced/23-json.html</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 23 we're going to talk about working with json.
+https://learn.massstreet.net/python/advanced/23-json.html
+</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>'Lesson File Xref'!A37</f>
+        <v>advanced</v>
+      </c>
+      <c r="B25" s="16">
+        <f>'Lesson File Xref'!C37</f>
+        <v>24</v>
+      </c>
+      <c r="C25" t="str">
+        <f>LOWER('Lesson File Xref'!D37)</f>
+        <v>making file request over http and ftp</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 24 we're going to talk about</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 24 we're going to talk about making file request over http and ftp.</v>
+      </c>
+      <c r="F25" t="str">
+        <f>'Lesson File Xref'!L37</f>
+        <v>https://learn.massstreet.net/python/advanced/24-requesting-files-with-http-ftp.html</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 24 we're going to talk about making file request over http and ftp.
+https://learn.massstreet.net/python/advanced/24-requesting-files-with-http-ftp.html
+</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>'Lesson File Xref'!A38</f>
+        <v>advanced</v>
+      </c>
+      <c r="B26" s="16">
+        <f>'Lesson File Xref'!C38</f>
+        <v>25</v>
+      </c>
+      <c r="C26" t="str">
+        <f>LOWER('Lesson File Xref'!D38)</f>
+        <v>interacting with databases</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 25 we're going to talk about</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 25 we're going to talk about interacting with databases.</v>
+      </c>
+      <c r="F26" t="str">
+        <f>'Lesson File Xref'!L38</f>
+        <v>https://learn.massstreet.net/python/advanced/25-databases.html</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 25 we're going to talk about interacting with databases.
+https://learn.massstreet.net/python/advanced/25-databases.html
+</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>'Lesson File Xref'!A39</f>
+        <v>advanced</v>
+      </c>
+      <c r="B27" s="16">
+        <f>'Lesson File Xref'!C39</f>
+        <v>26</v>
+      </c>
+      <c r="C27" t="str">
+        <f>LOWER('Lesson File Xref'!D39)</f>
+        <v>saving objects with pickle</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 26 we're going to talk about</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 26 we're going to talk about saving objects with pickle.</v>
+      </c>
+      <c r="F27" t="str">
+        <f>'Lesson File Xref'!L39</f>
+        <v>https://learn.massstreet.net/python/advanced/26-saving-objects-with-pickle.html</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 26 we're going to talk about saving objects with pickle.
+https://learn.massstreet.net/python/advanced/26-saving-objects-with-pickle.html
+</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>'Lesson File Xref'!A40</f>
+        <v>advanced</v>
+      </c>
+      <c r="B28" s="16">
+        <f>'Lesson File Xref'!C40</f>
+        <v>27</v>
+      </c>
+      <c r="C28" t="str">
+        <f>LOWER('Lesson File Xref'!D40)</f>
+        <v>error handling</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 27 we're going to talk about</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 27 we're going to talk about error handling.</v>
+      </c>
+      <c r="F28" t="str">
+        <f>'Lesson File Xref'!L40</f>
+        <v>https://learn.massstreet.net/python/advanced/27-error-handling.html</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 27 we're going to talk about error handling.
+https://learn.massstreet.net/python/advanced/27-error-handling.html
+</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f>'Lesson File Xref'!A41</f>
+        <v>advanced</v>
+      </c>
+      <c r="B29" s="16">
+        <f>'Lesson File Xref'!C41</f>
+        <v>28</v>
+      </c>
+      <c r="C29" t="str">
+        <f>LOWER('Lesson File Xref'!D41)</f>
+        <v>bringing it all together</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 28 we're going to talk about</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 28 we're going to talk about bringing it all together.</v>
+      </c>
+      <c r="F29" t="str">
+        <f>'Lesson File Xref'!L41</f>
+        <v>https://learn.massstreet.net/python/advanced/28-bringing-it-all-together.html</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 28 we're going to talk about bringing it all together.
+https://learn.massstreet.net/python/advanced/28-bringing-it-all-together.html
+</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f>'Lesson File Xref'!A42</f>
+        <v>solutions</v>
+      </c>
+      <c r="B30" s="16">
+        <f>'Lesson File Xref'!C42</f>
+        <v>29</v>
+      </c>
+      <c r="C30" t="str">
+        <f>LOWER('Lesson File Xref'!D42)</f>
+        <v>download a zip file over http</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 29 we're going to talk about</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 29 we're going to talk about download a zip file over http.</v>
+      </c>
+      <c r="F30" t="str">
+        <f>'Lesson File Xref'!L42</f>
+        <v>https://learn.massstreet.net/python/solutions/29-download-a-zip-file.html</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 29 we're going to talk about download a zip file over http.
+https://learn.massstreet.net/python/solutions/29-download-a-zip-file.html
+</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f>'Lesson File Xref'!A43</f>
+        <v>solutions</v>
+      </c>
+      <c r="B31" s="16">
+        <f>'Lesson File Xref'!C43</f>
+        <v>30</v>
+      </c>
+      <c r="C31" t="str">
+        <f>LOWER('Lesson File Xref'!D43)</f>
+        <v>looping over files in a directory</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 30 we're going to talk about</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 30 we're going to talk about looping over files in a directory.</v>
+      </c>
+      <c r="F31" t="str">
+        <f>'Lesson File Xref'!L43</f>
+        <v>https://learn.massstreet.net/python/solutions/30-looping-over-files-in-a-directory.html</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 30 we're going to talk about looping over files in a directory.
+https://learn.massstreet.net/python/solutions/30-looping-over-files-in-a-directory.html
+</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f>'Lesson File Xref'!A44</f>
+        <v>solutions</v>
+      </c>
+      <c r="B32" s="16">
+        <f>'Lesson File Xref'!C44</f>
+        <v>31</v>
+      </c>
+      <c r="C32" t="str">
+        <f>LOWER('Lesson File Xref'!D44)</f>
+        <v>convert comma delmited files to pipe delimited</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 31 we're going to talk about</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 31 we're going to talk about convert comma delmited files to pipe delimited.</v>
+      </c>
+      <c r="F32" t="str">
+        <f>'Lesson File Xref'!L44</f>
+        <v>https://learn.massstreet.net/python/solutions/31-convert-file-to-pipe-delimited.html</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 31 we're going to talk about convert comma delmited files to pipe delimited.
+https://learn.massstreet.net/python/solutions/31-convert-file-to-pipe-delimited.html
+</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>'Lesson File Xref'!A45</f>
+        <v>solutions</v>
+      </c>
+      <c r="B33" s="16">
+        <f>'Lesson File Xref'!C45</f>
+        <v>32</v>
+      </c>
+      <c r="C33" t="str">
+        <f>LOWER('Lesson File Xref'!D45)</f>
+        <v>combining multiple csvs into one file</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 32 we're going to talk about</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 32 we're going to talk about combining multiple csvs into one file.</v>
+      </c>
+      <c r="F33" t="str">
+        <f>'Lesson File Xref'!L45</f>
+        <v>https://learn.massstreet.net/python/solutions/32-combine-csvs-into-one-file.html</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 32 we're going to talk about combining multiple csvs into one file.
+https://learn.massstreet.net/python/solutions/32-combine-csvs-into-one-file.html
+</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f>'Lesson File Xref'!A46</f>
+        <v>solutions</v>
+      </c>
+      <c r="B34" s="16">
+        <f>'Lesson File Xref'!C46</f>
+        <v>33</v>
+      </c>
+      <c r="C34" t="str">
+        <f>LOWER('Lesson File Xref'!D46)</f>
+        <v>load large csvs into data warehouse staging tables</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 33 we're going to talk about</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 33 we're going to talk about load large csvs into data warehouse staging tables.</v>
+      </c>
+      <c r="F34" t="str">
+        <f>'Lesson File Xref'!L46</f>
+        <v>https://learn.massstreet.net/python/solutions/33-load-large-csvs-into-data-warehouse.html</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 33 we're going to talk about load large csvs into data warehouse staging tables.
+https://learn.massstreet.net/python/solutions/33-load-large-csvs-into-data-warehouse.html
+</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f>'Lesson File Xref'!A47</f>
+        <v>solutions</v>
+      </c>
+      <c r="B35" s="16">
+        <f>'Lesson File Xref'!C47</f>
+        <v>34</v>
+      </c>
+      <c r="C35" t="str">
+        <f>LOWER('Lesson File Xref'!D47)</f>
+        <v>efficiently write large database query results to disk</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 34 we're going to talk about</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 34 we're going to talk about efficiently write large database query results to disk.</v>
+      </c>
+      <c r="F35" t="str">
+        <f>'Lesson File Xref'!L47</f>
+        <v>https://learn.massstreet.net/python/solutions/34-efficient-disk-write.html</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 34 we're going to talk about efficiently write large database query results to disk.
+https://learn.massstreet.net/python/solutions/34-efficient-disk-write.html
+</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f>'Lesson File Xref'!A48</f>
+        <v>solutions</v>
+      </c>
+      <c r="B36" s="16">
+        <f>'Lesson File Xref'!C48</f>
+        <v>35</v>
+      </c>
+      <c r="C36" t="str">
+        <f>LOWER('Lesson File Xref'!D48)</f>
+        <v>working with sftp in the real world</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 35 we're going to talk about</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 35 we're going to talk about working with sftp in the real world.</v>
+      </c>
+      <c r="F36" t="str">
+        <f>'Lesson File Xref'!L48</f>
+        <v>https://learn.massstreet.net/python/solutions/35-sftp-in-the-real-world.html</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 35 we're going to talk about working with sftp in the real world.
+https://learn.massstreet.net/python/solutions/35-sftp-in-the-real-world.html
+</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f>'Lesson File Xref'!A49</f>
+        <v>solutions</v>
+      </c>
+      <c r="B37" s="16">
+        <f>'Lesson File Xref'!C49</f>
+        <v>36</v>
+      </c>
+      <c r="C37" t="str">
+        <f>LOWER('Lesson File Xref'!D49)</f>
+        <v>executing python from sql server agent</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="2"/>
+        <v>Here is your daily #Python lesson! Today in lesson 36 we're going to talk about</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="0"/>
+        <v>Here is your daily #Python lesson! Today in lesson 36 we're going to talk about executing python from sql server agent.</v>
+      </c>
+      <c r="F37" t="str">
+        <f>'Lesson File Xref'!L49</f>
+        <v>https://learn.massstreet.net/python/solutions/36-run-python-from-sql-server.html</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Here is your daily #Python lesson! Today in lesson 36 we're going to talk about executing python from sql server agent.
+https://learn.massstreet.net/python/solutions/36-run-python-from-sql-server.html
+</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02720D5E-A20F-4CFA-8B9E-1EE48C4E0140}">
   <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="G40" sqref="G39:G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7664,7 +9286,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294EA8A1-0E7E-44A0-A6A4-77513EA2BCD5}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -7692,7 +9314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E2A746-8891-4393-B508-2B889EC92277}">
   <dimension ref="A1:B7"/>
   <sheetViews>

</xml_diff>